<commit_message>
Fixed minor changes in the F matrix
</commit_message>
<xml_diff>
--- a/data/F.xlsx
+++ b/data/F.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/tmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\songc\Documents\NTNU\Emner\5. året\TKP4900 Master\JuMP Model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044CC9EE-277A-4821-A5C2-23B89B51CC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
   <si>
     <t>Variable</t>
   </si>
@@ -647,7 +647,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -945,11 +945,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="G178" sqref="G178"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.59765625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -966,7 +971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -974,67 +979,67 @@
         <v>113.76095996921192</v>
       </c>
       <c r="C2">
-        <v>4.6971578963950364e-5</v>
+        <v>4.6971578963950364E-5</v>
       </c>
       <c r="D2">
-        <v>4.840411989265054e-5</v>
+        <v>4.8404119892650542E-5</v>
       </c>
       <c r="E2">
-        <v>-4.02484937445971e-8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>-4.0248493744597103E-8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
-        <v>-1.0798671662802532e-44</v>
+        <v>-1.0798671662802532E-44</v>
       </c>
       <c r="C3">
-        <v>-5.368107533750759e-36</v>
+        <v>-5.3681075337507593E-36</v>
       </c>
       <c r="D3">
-        <v>3.153992141543457e-33</v>
+        <v>3.1539921415434568E-33</v>
       </c>
       <c r="E3">
-        <v>-2.7795515648053547e-36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>-2.7795515648053547E-36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
-        <v>1.3577067628692752e-43</v>
+        <v>1.3577067628692752E-43</v>
       </c>
       <c r="C4">
-        <v>1.4648995799039157e-34</v>
+        <v>1.4648995799039157E-34</v>
       </c>
       <c r="D4">
-        <v>-6.44143208502859e-26</v>
+        <v>-6.4414320850285898E-26</v>
       </c>
       <c r="E4">
-        <v>7.603698023557395e-35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>7.6036980235573947E-35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5">
-        <v>-3.8892624661201705e-42</v>
+        <v>-3.8892624661201705E-42</v>
       </c>
       <c r="C5">
-        <v>-7.057046565580051e-38</v>
+        <v>-7.0570465655800507E-38</v>
       </c>
       <c r="D5">
-        <v>-2.1154740576433757e-25</v>
+        <v>-2.1154740576433757E-25</v>
       </c>
       <c r="E5">
-        <v>9.140816387171898e-38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>9.1408163871718978E-38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1042,50 +1047,50 @@
         <v>1.9483599994726992</v>
       </c>
       <c r="C6">
-        <v>8.044723134982268e-7</v>
+        <v>8.0447231349822682E-7</v>
       </c>
       <c r="D6">
-        <v>8.289280266984888e-7</v>
+        <v>8.2892802669848882E-7</v>
       </c>
       <c r="E6">
-        <v>-6.858815218150862e-10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>-6.858815218150862E-10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7">
-        <v>8.8693999975996</v>
+        <v>8.8693999975996007</v>
       </c>
       <c r="C7">
-        <v>3.6621496507690296e-6</v>
+        <v>3.6621496507690296E-6</v>
       </c>
       <c r="D7">
-        <v>3.7735635515709186e-6</v>
+        <v>3.7735635515709186E-6</v>
       </c>
       <c r="E7">
-        <v>-3.144278252554776e-9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>-3.1442782525547759E-9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8">
-        <v>9.741799997363495</v>
+        <v>9.7417999973634952</v>
       </c>
       <c r="C8">
-        <v>4.022361872917419e-6</v>
+        <v>4.0223618729174193E-6</v>
       </c>
       <c r="D8">
-        <v>4.145274547199823e-6</v>
+        <v>4.1452745471998227E-6</v>
       </c>
       <c r="E8">
-        <v>-3.363066227850484e-9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>-3.3630662278504839E-9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1093,16 +1098,16 @@
         <v>3.6059199990240995</v>
       </c>
       <c r="C9">
-        <v>1.4888744971323444e-6</v>
+        <v>1.4888744971323444E-6</v>
       </c>
       <c r="D9">
-        <v>1.5344810644875359e-6</v>
+        <v>1.5344810644875359E-6</v>
       </c>
       <c r="E9">
-        <v>-1.2634516469754283e-9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>-1.2634516469754283E-9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1110,33 +1115,33 @@
         <v>2.0501399994451535</v>
       </c>
       <c r="C10">
-        <v>8.464970116638638e-7</v>
+        <v>8.4649701166386379E-7</v>
       </c>
       <c r="D10">
-        <v>8.719982503618091e-7</v>
+        <v>8.7199825036180915E-7</v>
       </c>
       <c r="E10">
-        <v>-7.105222341457867e-10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>-7.1052223414578668E-10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11">
-        <v>5.336179998555825</v>
+        <v>5.3361799985558251</v>
       </c>
       <c r="C11">
-        <v>2.2032943659455907e-6</v>
+        <v>2.2032943659455907E-6</v>
       </c>
       <c r="D11">
-        <v>2.270798547788992e-6</v>
+        <v>2.270798547788992E-6</v>
       </c>
       <c r="E11">
-        <v>-1.8548313448602313e-9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>-1.8548313448602313E-9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1144,67 +1149,67 @@
         <v>113.76095996921192</v>
       </c>
       <c r="C12">
-        <v>4.6971578963950364e-5</v>
+        <v>4.6971578963950364E-5</v>
       </c>
       <c r="D12">
-        <v>4.840411989265054e-5</v>
+        <v>4.8404119892650542E-5</v>
       </c>
       <c r="E12">
-        <v>-4.02484937445971e-8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>-4.0248493744597103E-8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13">
-        <v>716.8219938295638</v>
+        <v>716.82199382956378</v>
       </c>
       <c r="C13">
-        <v>0.0034684914754603167</v>
+        <v>3.4684914754603167E-3</v>
       </c>
       <c r="D13">
         <v>0.34907069314935024</v>
       </c>
       <c r="E13">
-        <v>-0.00034258103152575114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>-3.4258103152575114E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14">
-        <v>2.0549998498816777e-43</v>
+        <v>2.0549998498816777E-43</v>
       </c>
       <c r="C14">
-        <v>-7.322966611042391e-35</v>
+        <v>-7.3229666110423908E-35</v>
       </c>
       <c r="D14">
-        <v>-3.2207074370080907e-26</v>
+        <v>-3.2207074370080907E-26</v>
       </c>
       <c r="E14">
-        <v>-3.7874616981304386e-35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>-3.7874616981304386E-35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15">
-        <v>2.083252539316061e-42</v>
+        <v>2.083252539316061E-42</v>
       </c>
       <c r="C15">
-        <v>-1.2901630370691447e-34</v>
+        <v>-1.2901630370691447E-34</v>
       </c>
       <c r="D15">
-        <v>-9.67795893376539e-26</v>
+        <v>-9.6779589337653902E-26</v>
       </c>
       <c r="E15">
-        <v>-6.679847871565367e-35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>-6.6798478715653673E-35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1212,50 +1217,50 @@
         <v>1.9483599994726992</v>
       </c>
       <c r="C16">
-        <v>8.044723134982268e-7</v>
+        <v>8.0447231349822682E-7</v>
       </c>
       <c r="D16">
-        <v>8.289280266984888e-7</v>
+        <v>8.2892802669848882E-7</v>
       </c>
       <c r="E16">
-        <v>-6.858815218150862e-10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>-6.858815218150862E-10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17">
-        <v>8.8693999975996</v>
+        <v>8.8693999975996007</v>
       </c>
       <c r="C17">
-        <v>3.6621496507690296e-6</v>
+        <v>3.6621496507690296E-6</v>
       </c>
       <c r="D17">
-        <v>3.7735635515709186e-6</v>
+        <v>3.7735635515709186E-6</v>
       </c>
       <c r="E17">
-        <v>-3.144278252554776e-9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>-3.1442782525547759E-9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="B18">
-        <v>9.741799997363495</v>
+        <v>9.7417999973634952</v>
       </c>
       <c r="C18">
-        <v>4.022361872917419e-6</v>
+        <v>4.0223618729174193E-6</v>
       </c>
       <c r="D18">
-        <v>4.145274547199823e-6</v>
+        <v>4.1452745471998227E-6</v>
       </c>
       <c r="E18">
-        <v>-3.363066227850484e-9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>-3.3630662278504839E-9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1263,16 +1268,16 @@
         <v>3.6059199990240995</v>
       </c>
       <c r="C19">
-        <v>1.4888744971323444e-6</v>
+        <v>1.4888744971323444E-6</v>
       </c>
       <c r="D19">
-        <v>1.5344810644875359e-6</v>
+        <v>1.5344810644875359E-6</v>
       </c>
       <c r="E19">
-        <v>-1.2634516469754283e-9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>-1.2634516469754283E-9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1280,33 +1285,33 @@
         <v>2.0501399994451535</v>
       </c>
       <c r="C20">
-        <v>8.464970116638638e-7</v>
+        <v>8.4649701166386379E-7</v>
       </c>
       <c r="D20">
-        <v>8.719982503618091e-7</v>
+        <v>8.7199825036180915E-7</v>
       </c>
       <c r="E20">
-        <v>-7.105222341457867e-10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>-7.1052223414578668E-10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
       <c r="B21">
-        <v>5.336179998555825</v>
+        <v>5.3361799985558251</v>
       </c>
       <c r="C21">
-        <v>2.2032943659455907e-6</v>
+        <v>2.2032943659455907E-6</v>
       </c>
       <c r="D21">
-        <v>2.270798547788992e-6</v>
+        <v>2.270798547788992E-6</v>
       </c>
       <c r="E21">
-        <v>-1.8548313448602313e-9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>-1.8548313448602313E-9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1314,67 +1319,67 @@
         <v>113.76095996921192</v>
       </c>
       <c r="C22">
-        <v>4.6971578963950364e-5</v>
+        <v>4.6971578963950364E-5</v>
       </c>
       <c r="D22">
-        <v>4.840411989265054e-5</v>
+        <v>4.8404119892650542E-5</v>
       </c>
       <c r="E22">
-        <v>-4.02484937445971e-8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>-4.0248493744597103E-8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
       <c r="B23">
-        <v>716.8219938295638</v>
+        <v>716.82199382956378</v>
       </c>
       <c r="C23">
-        <v>0.0034684914754603167</v>
+        <v>3.4684914754603167E-3</v>
       </c>
       <c r="D23">
         <v>0.34907069314935024</v>
       </c>
       <c r="E23">
-        <v>-0.00034258103152575114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>-3.4258103152575114E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>27</v>
       </c>
       <c r="B24">
-        <v>2.1014708141234524e-42</v>
+        <v>2.1014708141234524E-42</v>
       </c>
       <c r="C24">
-        <v>-3.4293919571991376e-38</v>
+        <v>-3.4293919571991376E-38</v>
       </c>
       <c r="D24">
-        <v>-5.30470168624217e-26</v>
+        <v>-5.3047016862421695E-26</v>
       </c>
       <c r="E24">
-        <v>-3.0090309171974163e-37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>-3.0090309171974163E-37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>28</v>
       </c>
       <c r="B25">
-        <v>3.6424306022568e-42</v>
+        <v>3.6424306022568E-42</v>
       </c>
       <c r="C25">
-        <v>-2.579662825789951e-34</v>
+        <v>-2.5796628257899508E-34</v>
       </c>
       <c r="D25">
-        <v>2.66979902912764e-26</v>
+        <v>2.6697990291276402E-26</v>
       </c>
       <c r="E25">
-        <v>-1.3354098108927875e-34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>-1.3354098108927875E-34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1382,50 +1387,50 @@
         <v>1.9483599994726992</v>
       </c>
       <c r="C26">
-        <v>8.044723134982268e-7</v>
+        <v>8.0447231349822682E-7</v>
       </c>
       <c r="D26">
-        <v>8.289280266984888e-7</v>
+        <v>8.2892802669848882E-7</v>
       </c>
       <c r="E26">
-        <v>-6.858815218150862e-10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>-6.858815218150862E-10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>30</v>
       </c>
       <c r="B27">
-        <v>8.8693999975996</v>
+        <v>8.8693999975996007</v>
       </c>
       <c r="C27">
-        <v>3.6621496507690296e-6</v>
+        <v>3.6621496507690296E-6</v>
       </c>
       <c r="D27">
-        <v>3.7735635515709186e-6</v>
+        <v>3.7735635515709186E-6</v>
       </c>
       <c r="E27">
-        <v>-3.144278252554776e-9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>-3.1442782525547759E-9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
       <c r="B28">
-        <v>9.741799997363495</v>
+        <v>9.7417999973634952</v>
       </c>
       <c r="C28">
-        <v>4.022361872917419e-6</v>
+        <v>4.0223618729174193E-6</v>
       </c>
       <c r="D28">
-        <v>4.145274547199823e-6</v>
+        <v>4.1452745471998227E-6</v>
       </c>
       <c r="E28">
-        <v>-3.363066227850484e-9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>-3.3630662278504839E-9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1433,16 +1438,16 @@
         <v>3.6059199990240995</v>
       </c>
       <c r="C29">
-        <v>1.4888744971323444e-6</v>
+        <v>1.4888744971323444E-6</v>
       </c>
       <c r="D29">
-        <v>1.5344810644875359e-6</v>
+        <v>1.5344810644875359E-6</v>
       </c>
       <c r="E29">
-        <v>-1.2634516469754283e-9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>-1.2634516469754283E-9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1450,33 +1455,33 @@
         <v>2.0501399994451535</v>
       </c>
       <c r="C30">
-        <v>8.464970116638638e-7</v>
+        <v>8.4649701166386379E-7</v>
       </c>
       <c r="D30">
-        <v>8.719982503618091e-7</v>
+        <v>8.7199825036180915E-7</v>
       </c>
       <c r="E30">
-        <v>-7.105222341457867e-10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>-7.1052223414578668E-10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>34</v>
       </c>
       <c r="B31">
-        <v>5.336179998555825</v>
+        <v>5.3361799985558251</v>
       </c>
       <c r="C31">
-        <v>2.2032943659455907e-6</v>
+        <v>2.2032943659455907E-6</v>
       </c>
       <c r="D31">
-        <v>2.270798547788992e-6</v>
+        <v>2.270798547788992E-6</v>
       </c>
       <c r="E31">
-        <v>-1.8548313448602313e-9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>-1.8548313448602313E-9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1484,67 +1489,67 @@
         <v>113.76095996921192</v>
       </c>
       <c r="C32">
-        <v>4.6971578963950364e-5</v>
+        <v>4.6971578963950364E-5</v>
       </c>
       <c r="D32">
-        <v>4.840411989265054e-5</v>
+        <v>4.8404119892650542E-5</v>
       </c>
       <c r="E32">
-        <v>-4.02484937445971e-8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>-4.0248493744597103E-8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>36</v>
       </c>
       <c r="B33">
-        <v>716.8219938295638</v>
+        <v>716.82199382956378</v>
       </c>
       <c r="C33">
-        <v>0.0034684914754603167</v>
+        <v>3.4684914754603167E-3</v>
       </c>
       <c r="D33">
         <v>0.34907069314935024</v>
       </c>
       <c r="E33">
-        <v>-0.00034258103152575114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>-3.4258103152575114E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>37</v>
       </c>
       <c r="B34">
-        <v>1.7695986017706285e-42</v>
+        <v>1.7695986017706285E-42</v>
       </c>
       <c r="C34">
-        <v>3.66096305287079e-35</v>
+        <v>3.6609630528707902E-35</v>
       </c>
       <c r="D34">
-        <v>9.472466512141533e-28</v>
+        <v>9.4724665121415325E-28</v>
       </c>
       <c r="E34">
-        <v>1.881620541681442e-35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>1.881620541681442E-35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>38</v>
       </c>
       <c r="B35">
-        <v>-1.2378175786874966e-42</v>
+        <v>-1.2378175786874966E-42</v>
       </c>
       <c r="C35">
-        <v>-2.6903027677569266e-34</v>
+        <v>-2.6903027677569266E-34</v>
       </c>
       <c r="D35">
-        <v>-2.2272026306163275e-25</v>
+        <v>-2.2272026306163275E-25</v>
       </c>
       <c r="E35">
-        <v>-1.390862291978149e-34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>-1.390862291978149E-34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1552,50 +1557,50 @@
         <v>1.9483599994726992</v>
       </c>
       <c r="C36">
-        <v>8.044723134982268e-7</v>
+        <v>8.0447231349822682E-7</v>
       </c>
       <c r="D36">
-        <v>8.289280266984888e-7</v>
+        <v>8.2892802669848882E-7</v>
       </c>
       <c r="E36">
-        <v>-6.858815218150862e-10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>-6.858815218150862E-10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>40</v>
       </c>
       <c r="B37">
-        <v>8.8693999975996</v>
+        <v>8.8693999975996007</v>
       </c>
       <c r="C37">
-        <v>3.6621496507690296e-6</v>
+        <v>3.6621496507690296E-6</v>
       </c>
       <c r="D37">
-        <v>3.7735635515709186e-6</v>
+        <v>3.7735635515709186E-6</v>
       </c>
       <c r="E37">
-        <v>-3.144278252554776e-9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>-3.1442782525547759E-9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>41</v>
       </c>
       <c r="B38">
-        <v>9.741799997363495</v>
+        <v>9.7417999973634952</v>
       </c>
       <c r="C38">
-        <v>4.022361872917419e-6</v>
+        <v>4.0223618729174193E-6</v>
       </c>
       <c r="D38">
-        <v>4.145274547199823e-6</v>
+        <v>4.1452745471998227E-6</v>
       </c>
       <c r="E38">
-        <v>-3.363066227850484e-9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>-3.3630662278504839E-9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1603,16 +1608,16 @@
         <v>3.6059199990240995</v>
       </c>
       <c r="C39">
-        <v>1.4888744971323444e-6</v>
+        <v>1.4888744971323444E-6</v>
       </c>
       <c r="D39">
-        <v>1.5344810644875359e-6</v>
+        <v>1.5344810644875359E-6</v>
       </c>
       <c r="E39">
-        <v>-1.2634516469754283e-9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>-1.2634516469754283E-9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -1620,33 +1625,33 @@
         <v>2.0501399994451535</v>
       </c>
       <c r="C40">
-        <v>8.464970116638638e-7</v>
+        <v>8.4649701166386379E-7</v>
       </c>
       <c r="D40">
-        <v>8.719982503618091e-7</v>
+        <v>8.7199825036180915E-7</v>
       </c>
       <c r="E40">
-        <v>-7.105222341457867e-10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>-7.1052223414578668E-10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>44</v>
       </c>
       <c r="B41">
-        <v>5.336179998555825</v>
+        <v>5.3361799985558251</v>
       </c>
       <c r="C41">
-        <v>2.2032943659455907e-6</v>
+        <v>2.2032943659455907E-6</v>
       </c>
       <c r="D41">
-        <v>2.270798547788992e-6</v>
+        <v>2.270798547788992E-6</v>
       </c>
       <c r="E41">
-        <v>-1.8548313448602313e-9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>-1.8548313448602313E-9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -1654,67 +1659,67 @@
         <v>113.76095996921192</v>
       </c>
       <c r="C42">
-        <v>4.6971578963950364e-5</v>
+        <v>4.6971578963950364E-5</v>
       </c>
       <c r="D42">
-        <v>4.840411989265054e-5</v>
+        <v>4.8404119892650542E-5</v>
       </c>
       <c r="E42">
-        <v>-4.02484937445971e-8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>-4.0248493744597103E-8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>46</v>
       </c>
       <c r="B43">
-        <v>716.8219938295638</v>
+        <v>716.82199382956378</v>
       </c>
       <c r="C43">
-        <v>0.0034684914754603167</v>
+        <v>3.4684914754603167E-3</v>
       </c>
       <c r="D43">
         <v>0.34907069314935024</v>
       </c>
       <c r="E43">
-        <v>-0.00034258103152575114</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>-3.4258103152575114E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>47</v>
       </c>
       <c r="B44">
-        <v>9.763189785065321e-43</v>
+        <v>9.7631897850653208E-43</v>
       </c>
       <c r="C44">
-        <v>-1.46482483590846e-34</v>
+        <v>-1.4648248359084601E-34</v>
       </c>
       <c r="D44">
-        <v>6.062524819118722e-26</v>
+        <v>6.0625248191187222E-26</v>
       </c>
       <c r="E44">
-        <v>-7.57543294383245e-35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>-7.5754329438324499E-35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>48</v>
       </c>
       <c r="B45">
-        <v>7.89677127326731e-43</v>
+        <v>7.89677127326731E-43</v>
       </c>
       <c r="C45">
-        <v>-8.070814617304614e-34</v>
+        <v>-8.0708146173046137E-34</v>
       </c>
       <c r="D45">
-        <v>-8.351968370042896e-26</v>
+        <v>-8.3519683700428957E-26</v>
       </c>
       <c r="E45">
-        <v>-4.1739557797938e-34</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>-4.1739557797937996E-34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -1722,50 +1727,50 @@
         <v>1.9483599994726992</v>
       </c>
       <c r="C46">
-        <v>8.044723134982268e-7</v>
+        <v>8.0447231349822682E-7</v>
       </c>
       <c r="D46">
-        <v>8.289280266984888e-7</v>
+        <v>8.2892802669848882E-7</v>
       </c>
       <c r="E46">
-        <v>-6.858815218150862e-10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>-6.858815218150862E-10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>50</v>
       </c>
       <c r="B47">
-        <v>8.8693999975996</v>
+        <v>8.8693999975996007</v>
       </c>
       <c r="C47">
-        <v>3.6621496507690296e-6</v>
+        <v>3.6621496507690296E-6</v>
       </c>
       <c r="D47">
-        <v>3.7735635515709186e-6</v>
+        <v>3.7735635515709186E-6</v>
       </c>
       <c r="E47">
-        <v>-3.144278252554776e-9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>-3.1442782525547759E-9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>51</v>
       </c>
       <c r="B48">
-        <v>9.741799997363495</v>
+        <v>9.7417999973634952</v>
       </c>
       <c r="C48">
-        <v>4.022361872917419e-6</v>
+        <v>4.0223618729174193E-6</v>
       </c>
       <c r="D48">
-        <v>4.145274547199823e-6</v>
+        <v>4.1452745471998227E-6</v>
       </c>
       <c r="E48">
-        <v>-3.363066227850484e-9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>-3.3630662278504839E-9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1773,16 +1778,16 @@
         <v>3.6059199990240995</v>
       </c>
       <c r="C49">
-        <v>1.4888744971323444e-6</v>
+        <v>1.4888744971323444E-6</v>
       </c>
       <c r="D49">
-        <v>1.5344810644875359e-6</v>
+        <v>1.5344810644875359E-6</v>
       </c>
       <c r="E49">
-        <v>-1.2634516469754283e-9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>-1.2634516469754283E-9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -1790,33 +1795,33 @@
         <v>2.0501399994451535</v>
       </c>
       <c r="C50">
-        <v>8.464970116638638e-7</v>
+        <v>8.4649701166386379E-7</v>
       </c>
       <c r="D50">
-        <v>8.719982503618091e-7</v>
+        <v>8.7199825036180915E-7</v>
       </c>
       <c r="E50">
-        <v>-7.105222341457867e-10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>-7.1052223414578668E-10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>54</v>
       </c>
       <c r="B51">
-        <v>5.336179998555825</v>
+        <v>5.3361799985558251</v>
       </c>
       <c r="C51">
-        <v>2.2032943659455907e-6</v>
+        <v>2.2032943659455907E-6</v>
       </c>
       <c r="D51">
-        <v>2.270798547788992e-6</v>
+        <v>2.270798547788992E-6</v>
       </c>
       <c r="E51">
-        <v>-1.8548313448602313e-9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>-1.8548313448602313E-9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -1824,33 +1829,33 @@
         <v>179.52172526328644</v>
       </c>
       <c r="C52">
-        <v>3.259598334038693e-5</v>
+        <v>3.259598334038693E-5</v>
       </c>
       <c r="D52">
-        <v>-0.004454707914659524</v>
+        <v>-4.4547079146595239E-3</v>
       </c>
       <c r="E52">
-        <v>4.399172902243834e-6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+        <v>4.399172902243834E-6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>56</v>
       </c>
       <c r="B53">
-        <v>656.0326960970309</v>
+        <v>656.03269609703091</v>
       </c>
       <c r="C53">
-        <v>0.0033601090013836445</v>
+        <v>3.3601090013836445E-3</v>
       </c>
       <c r="D53">
-        <v>0.3399564522509702</v>
+        <v>0.33995645225097021</v>
       </c>
       <c r="E53">
-        <v>-0.0003336078933058784</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>-3.3360789330587841E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -1858,16 +1863,16 @@
         <v>55.140547110317776</v>
       </c>
       <c r="C54">
-        <v>0.0001891062352918736</v>
+        <v>1.8910623529187361E-4</v>
       </c>
       <c r="D54">
-        <v>0.018174136552332392</v>
+        <v>1.8174136552332392E-2</v>
       </c>
       <c r="E54">
-        <v>-1.789376858114436e-5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+        <v>-1.7893768581144359E-5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -1875,118 +1880,118 @@
         <v>0.22785162720980615</v>
       </c>
       <c r="C55">
-        <v>-1.326471962948949e-7</v>
+        <v>-1.326471962948949E-7</v>
       </c>
       <c r="D55">
-        <v>-2.6176277646587095e-5</v>
+        <v>-2.6176277646587095E-5</v>
       </c>
       <c r="E55">
-        <v>2.5124156933715828e-8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+        <v>2.5124156933715828E-8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>59</v>
       </c>
       <c r="B56">
-        <v>32.22908305213422</v>
+        <v>32.229083052134222</v>
       </c>
       <c r="C56">
-        <v>5.506204432710169e-5</v>
+        <v>5.5062044327101691E-5</v>
       </c>
       <c r="D56">
-        <v>0.004571072963843211</v>
+        <v>4.5710729638432108E-3</v>
       </c>
       <c r="E56">
-        <v>-4.499435192315728e-6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+        <v>-4.4994351923157284E-6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>60</v>
       </c>
       <c r="B57">
-        <v>7.073072359994564e-17</v>
+        <v>7.0730723599945638E-17</v>
       </c>
       <c r="C57">
-        <v>-1.5806407997613857e-13</v>
+        <v>-1.5806407997613857E-13</v>
       </c>
       <c r="D57">
-        <v>2.705665452844661e-11</v>
+        <v>2.7056654528446611E-11</v>
       </c>
       <c r="E57">
-        <v>2.015876925872519e-11</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+        <v>2.0158769258725188E-11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>61</v>
       </c>
       <c r="B58">
-        <v>7.073072359994561e-17</v>
+        <v>7.0730723599945613E-17</v>
       </c>
       <c r="C58">
-        <v>-2.202204832463742e-13</v>
+        <v>-2.202204832463742E-13</v>
       </c>
       <c r="D58">
-        <v>-4.906840013125181e-10</v>
+        <v>-4.9068400131251812E-10</v>
       </c>
       <c r="E58">
-        <v>1.8802088481273723e-11</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+        <v>1.8802088481273723E-11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>62</v>
       </c>
       <c r="B59">
-        <v>4.348474418120851e-17</v>
+        <v>4.3484744181208512E-17</v>
       </c>
       <c r="C59">
-        <v>-1.206672050048402e-13</v>
+        <v>-1.2066720500484019E-13</v>
       </c>
       <c r="D59">
-        <v>8.759577505197369e-12</v>
+        <v>8.7595775051973687E-12</v>
       </c>
       <c r="E59">
-        <v>3.956193982091278e-12</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+        <v>3.9561939820912782E-12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>63</v>
       </c>
       <c r="B60">
-        <v>4.348474418120851e-17</v>
+        <v>4.3484744181208512E-17</v>
       </c>
       <c r="C60">
-        <v>-7.324733433515021e-14</v>
+        <v>-7.324733433515021E-14</v>
       </c>
       <c r="D60">
-        <v>-3.3002372003102834e-11</v>
+        <v>-3.3002372003102834E-11</v>
       </c>
       <c r="E60">
-        <v>-4.220164408345869e-12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+        <v>-4.2201644083458693E-12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>64</v>
       </c>
       <c r="B61">
-        <v>-4.384802850591589e-16</v>
+        <v>-4.3848028505915892E-16</v>
       </c>
       <c r="C61">
-        <v>3.4653697035623437e-13</v>
+        <v>3.4653697035623437E-13</v>
       </c>
       <c r="D61">
-        <v>1.910694672295929e-10</v>
+        <v>1.910694672295929E-10</v>
       </c>
       <c r="E61">
-        <v>3.0586160148583495e-12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+        <v>3.0586160148583495E-12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -1994,33 +1999,33 @@
         <v>179.52172526328644</v>
       </c>
       <c r="C62">
-        <v>3.259598334038693e-5</v>
+        <v>3.259598334038693E-5</v>
       </c>
       <c r="D62">
-        <v>-0.004454707914659524</v>
+        <v>-4.4547079146595239E-3</v>
       </c>
       <c r="E62">
-        <v>4.399172902243834e-6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+        <v>4.399172902243834E-6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>66</v>
       </c>
       <c r="B63">
-        <v>656.0326960970309</v>
+        <v>656.03269609703091</v>
       </c>
       <c r="C63">
-        <v>0.0033601090013836445</v>
+        <v>3.3601090013836445E-3</v>
       </c>
       <c r="D63">
-        <v>0.3399564522509702</v>
+        <v>0.33995645225097021</v>
       </c>
       <c r="E63">
-        <v>-0.0003336078933058784</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+        <v>-3.3360789330587841E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -2028,16 +2033,16 @@
         <v>55.140547110317776</v>
       </c>
       <c r="C64">
-        <v>0.0001891062352918736</v>
+        <v>1.8910623529187361E-4</v>
       </c>
       <c r="D64">
-        <v>0.018174136552332392</v>
+        <v>1.8174136552332392E-2</v>
       </c>
       <c r="E64">
-        <v>-1.789376858114436e-5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+        <v>-1.7893768581144359E-5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -2045,33 +2050,33 @@
         <v>0.22785162720980615</v>
       </c>
       <c r="C65">
-        <v>-1.326471962948949e-7</v>
+        <v>-1.326471962948949E-7</v>
       </c>
       <c r="D65">
-        <v>-2.6176277646587095e-5</v>
+        <v>-2.6176277646587095E-5</v>
       </c>
       <c r="E65">
-        <v>2.5124156933715828e-8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+        <v>2.5124156933715828E-8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>69</v>
       </c>
       <c r="B66">
-        <v>32.22908305213422</v>
+        <v>32.229083052134222</v>
       </c>
       <c r="C66">
-        <v>5.506204432710169e-5</v>
+        <v>5.5062044327101691E-5</v>
       </c>
       <c r="D66">
-        <v>0.004571072963843211</v>
+        <v>4.5710729638432108E-3</v>
       </c>
       <c r="E66">
-        <v>-4.499435192315728e-6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+        <v>-4.4994351923157284E-6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -2079,33 +2084,33 @@
         <v>179.52172526328644</v>
       </c>
       <c r="C67">
-        <v>3.259598334038693e-5</v>
+        <v>3.259598334038693E-5</v>
       </c>
       <c r="D67">
-        <v>-0.004454707914659524</v>
+        <v>-4.4547079146595239E-3</v>
       </c>
       <c r="E67">
-        <v>4.399172902243834e-6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+        <v>4.399172902243834E-6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>71</v>
       </c>
       <c r="B68">
-        <v>656.0326960970309</v>
+        <v>656.03269609703091</v>
       </c>
       <c r="C68">
-        <v>0.0033601090013836445</v>
+        <v>3.3601090013836445E-3</v>
       </c>
       <c r="D68">
-        <v>0.3399564522509702</v>
+        <v>0.33995645225097021</v>
       </c>
       <c r="E68">
-        <v>-0.0003336078933058784</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
+        <v>-3.3360789330587841E-4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>72</v>
       </c>
@@ -2113,16 +2118,16 @@
         <v>55.140547110317776</v>
       </c>
       <c r="C69">
-        <v>0.0001891062352918736</v>
+        <v>1.8910623529187361E-4</v>
       </c>
       <c r="D69">
-        <v>0.018174136552332392</v>
+        <v>1.8174136552332392E-2</v>
       </c>
       <c r="E69">
-        <v>-1.789376858114436e-5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
+        <v>-1.7893768581144359E-5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>73</v>
       </c>
@@ -2130,33 +2135,33 @@
         <v>0.22785162720980615</v>
       </c>
       <c r="C70">
-        <v>-1.326471962948949e-7</v>
+        <v>-1.326471962948949E-7</v>
       </c>
       <c r="D70">
-        <v>-2.6176277646587095e-5</v>
+        <v>-2.6176277646587095E-5</v>
       </c>
       <c r="E70">
-        <v>2.5124156933715828e-8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
+        <v>2.5124156933715828E-8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>74</v>
       </c>
       <c r="B71">
-        <v>32.22908305213422</v>
+        <v>32.229083052134222</v>
       </c>
       <c r="C71">
-        <v>5.506204432710169e-5</v>
+        <v>5.5062044327101691E-5</v>
       </c>
       <c r="D71">
-        <v>0.004571072963843211</v>
+        <v>4.5710729638432108E-3</v>
       </c>
       <c r="E71">
-        <v>-4.499435192315728e-6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
+        <v>-4.4994351923157284E-6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>75</v>
       </c>
@@ -2164,33 +2169,33 @@
         <v>179.52172526328644</v>
       </c>
       <c r="C72">
-        <v>3.259598334038693e-5</v>
+        <v>3.259598334038693E-5</v>
       </c>
       <c r="D72">
-        <v>-0.004454707914659524</v>
+        <v>-4.4547079146595239E-3</v>
       </c>
       <c r="E72">
-        <v>4.399172902243834e-6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
+        <v>4.399172902243834E-6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>76</v>
       </c>
       <c r="B73">
-        <v>656.0326960970309</v>
+        <v>656.03269609703091</v>
       </c>
       <c r="C73">
-        <v>0.0033601090013836445</v>
+        <v>3.3601090013836445E-3</v>
       </c>
       <c r="D73">
-        <v>0.3399564522509702</v>
+        <v>0.33995645225097021</v>
       </c>
       <c r="E73">
-        <v>-0.0003336078933058784</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
+        <v>-3.3360789330587841E-4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>77</v>
       </c>
@@ -2198,16 +2203,16 @@
         <v>55.140547110317776</v>
       </c>
       <c r="C74">
-        <v>0.0001891062352918736</v>
+        <v>1.8910623529187361E-4</v>
       </c>
       <c r="D74">
-        <v>0.018174136552332392</v>
+        <v>1.8174136552332392E-2</v>
       </c>
       <c r="E74">
-        <v>-1.789376858114436e-5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
+        <v>-1.7893768581144359E-5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>78</v>
       </c>
@@ -2215,67 +2220,67 @@
         <v>0.22785162720980615</v>
       </c>
       <c r="C75">
-        <v>-1.326471962948949e-7</v>
+        <v>-1.326471962948949E-7</v>
       </c>
       <c r="D75">
-        <v>-2.6176277646587095e-5</v>
+        <v>-2.6176277646587095E-5</v>
       </c>
       <c r="E75">
-        <v>2.5124156933715828e-8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
+        <v>2.5124156933715828E-8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>79</v>
       </c>
       <c r="B76">
-        <v>32.22908305213422</v>
+        <v>32.229083052134222</v>
       </c>
       <c r="C76">
-        <v>5.506204432710169e-5</v>
+        <v>5.5062044327101691E-5</v>
       </c>
       <c r="D76">
-        <v>0.004571072963843211</v>
+        <v>4.5710729638432108E-3</v>
       </c>
       <c r="E76">
-        <v>-4.499435192315728e-6</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
+        <v>-4.4994351923157284E-6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>80</v>
       </c>
       <c r="B77">
-        <v>94.62582114643622</v>
+        <v>94.625821146436223</v>
       </c>
       <c r="C77">
-        <v>-0.0002372949494924565</v>
+        <v>-2.3729494949245651E-4</v>
       </c>
       <c r="D77">
-        <v>-0.028720270960206594</v>
+        <v>-2.8720270960206594E-2</v>
       </c>
       <c r="E77">
-        <v>2.825088361775748e-5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
+        <v>2.8250883617757481E-5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>81</v>
       </c>
       <c r="B78">
-        <v>518.6180599623617</v>
+        <v>518.61805996236171</v>
       </c>
       <c r="C78">
-        <v>0.0028634557240236665</v>
+        <v>2.8634557240236665E-3</v>
       </c>
       <c r="D78">
-        <v>0.2934579861101063</v>
+        <v>0.29345798611010632</v>
       </c>
       <c r="E78">
-        <v>-0.0002879373046931402</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
+        <v>-2.8793730469314018E-4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>82</v>
       </c>
@@ -2283,84 +2288,84 @@
         <v>362.34699147868747</v>
       </c>
       <c r="C79">
-        <v>0.001225541285467987</v>
+        <v>1.2255412854679871E-3</v>
       </c>
       <c r="D79">
         <v>0.11320366788086986</v>
       </c>
       <c r="E79">
-        <v>-0.00011126692945545275</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
+        <v>-1.1126692945545275E-4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>83</v>
       </c>
       <c r="B80">
-        <v>32.605023726241</v>
+        <v>32.605023726241001</v>
       </c>
       <c r="C80">
-        <v>4.2996060683729675e-5</v>
+        <v>4.2996060683729675E-5</v>
       </c>
       <c r="D80">
-        <v>0.002006505401149147</v>
+        <v>2.0065054011491469E-3</v>
       </c>
       <c r="E80">
-        <v>-2.0096134882036183e-6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
+        <v>-2.0096134882036183E-6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>84</v>
       </c>
       <c r="B81">
-        <v>84.74781506995325</v>
+        <v>84.747815069953248</v>
       </c>
       <c r="C81">
-        <v>0.00028182426668380266</v>
+        <v>2.8182426668380266E-4</v>
       </c>
       <c r="D81">
-        <v>0.02680393545685095</v>
+        <v>2.680393545685095E-2</v>
       </c>
       <c r="E81">
-        <v>-2.6316614750290048e-5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
+        <v>-2.6316614750290048E-5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>85</v>
       </c>
       <c r="B82">
-        <v>94.62582114643622</v>
+        <v>94.625821146436223</v>
       </c>
       <c r="C82">
-        <v>-0.0002372949494924565</v>
+        <v>-2.3729494949245651E-4</v>
       </c>
       <c r="D82">
-        <v>-0.028720270960206594</v>
+        <v>-2.8720270960206594E-2</v>
       </c>
       <c r="E82">
-        <v>2.825088361775748e-5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
+        <v>2.8250883617757481E-5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>86</v>
       </c>
       <c r="B83">
-        <v>518.6180599623617</v>
+        <v>518.61805996236171</v>
       </c>
       <c r="C83">
-        <v>0.0028634557240236665</v>
+        <v>2.8634557240236665E-3</v>
       </c>
       <c r="D83">
-        <v>0.2934579861101063</v>
+        <v>0.29345798611010632</v>
       </c>
       <c r="E83">
-        <v>-0.0002879373046931402</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
+        <v>-2.8793730469314018E-4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>87</v>
       </c>
@@ -2368,50 +2373,50 @@
         <v>362.34699147868747</v>
       </c>
       <c r="C84">
-        <v>0.001225541285467987</v>
+        <v>1.2255412854679871E-3</v>
       </c>
       <c r="D84">
         <v>0.11320366788086986</v>
       </c>
       <c r="E84">
-        <v>-0.00011126692945545275</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
+        <v>-1.1126692945545275E-4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>88</v>
       </c>
       <c r="B85">
-        <v>32.605023726241</v>
+        <v>32.605023726241001</v>
       </c>
       <c r="C85">
-        <v>4.2996060683729675e-5</v>
+        <v>4.2996060683729675E-5</v>
       </c>
       <c r="D85">
-        <v>0.002006505401149147</v>
+        <v>2.0065054011491469E-3</v>
       </c>
       <c r="E85">
-        <v>-2.0096134882036183e-6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
+        <v>-2.0096134882036183E-6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>89</v>
       </c>
       <c r="B86">
-        <v>84.74781506995325</v>
+        <v>84.747815069953248</v>
       </c>
       <c r="C86">
-        <v>0.00028182426668380266</v>
+        <v>2.8182426668380266E-4</v>
       </c>
       <c r="D86">
-        <v>0.02680393545685095</v>
+        <v>2.680393545685095E-2</v>
       </c>
       <c r="E86">
-        <v>-2.6316614750290048e-5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
+        <v>-2.6316614750290048E-5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>90</v>
       </c>
@@ -2419,50 +2424,50 @@
         <v>0.30066254435730366</v>
       </c>
       <c r="C87">
-        <v>-2.851398607942417e-6</v>
+        <v>-2.851398607942417E-6</v>
       </c>
       <c r="D87">
-        <v>-0.000310175485918379</v>
+        <v>-3.1017548591837898E-4</v>
       </c>
       <c r="E87">
-        <v>3.0613332341107063e-7</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
+        <v>3.0613332341107063E-7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>91</v>
       </c>
       <c r="B88">
-        <v>582.9335734881603</v>
+        <v>582.93357348816028</v>
       </c>
       <c r="C88">
-        <v>0.0031237528626846486</v>
+        <v>3.1237528626846486E-3</v>
       </c>
       <c r="D88">
-        <v>0.3178366623302741</v>
+        <v>0.31783666233027408</v>
       </c>
       <c r="E88">
-        <v>-0.00031196662490986447</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
+        <v>-3.1196662490986447E-4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>92</v>
       </c>
       <c r="B89">
-        <v>486.6817951570467</v>
+        <v>486.68179515704668</v>
       </c>
       <c r="C89">
-        <v>0.0004963570979530794</v>
+        <v>4.9635709795307935E-4</v>
       </c>
       <c r="D89">
-        <v>0.03200487359035111</v>
+        <v>3.2004873590351111E-2</v>
       </c>
       <c r="E89">
-        <v>-3.134651645689342e-5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
+        <v>-3.134651645689342E-5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>93</v>
       </c>
@@ -2470,33 +2475,33 @@
         <v>126.9767299474213</v>
       </c>
       <c r="C90">
-        <v>-0.0001655368056910255</v>
+        <v>-1.6553680569102549E-4</v>
       </c>
       <c r="D90">
-        <v>-0.024533559874365854</v>
+        <v>-2.4533559874365854E-2</v>
       </c>
       <c r="E90">
-        <v>2.4052914168587593e-5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
+        <v>2.4052914168587593E-5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>94</v>
       </c>
       <c r="B91">
-        <v>84.70126745085186</v>
+        <v>84.701267450851859</v>
       </c>
       <c r="C91">
-        <v>0.00025591359885793034</v>
+        <v>2.5591359885793034E-4</v>
       </c>
       <c r="D91">
-        <v>0.02493392139591429</v>
+        <v>2.4933921395914289E-2</v>
       </c>
       <c r="E91">
-        <v>-2.4433808308527345e-5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
+        <v>-2.4433808308527345E-5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -2504,50 +2509,50 @@
         <v>0.30066254435730366</v>
       </c>
       <c r="C92">
-        <v>-2.851398607942417e-6</v>
+        <v>-2.851398607942417E-6</v>
       </c>
       <c r="D92">
-        <v>-0.000310175485918379</v>
+        <v>-3.1017548591837898E-4</v>
       </c>
       <c r="E92">
-        <v>3.0613332341107063e-7</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5">
+        <v>3.0613332341107063E-7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>96</v>
       </c>
       <c r="B93">
-        <v>582.9335734881603</v>
+        <v>582.93357348816028</v>
       </c>
       <c r="C93">
-        <v>0.0031237528626846486</v>
+        <v>3.1237528626846486E-3</v>
       </c>
       <c r="D93">
-        <v>0.3178366623302741</v>
+        <v>0.31783666233027408</v>
       </c>
       <c r="E93">
-        <v>-0.00031196662490986447</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
+        <v>-3.1196662490986447E-4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>97</v>
       </c>
       <c r="B94">
-        <v>486.6817951570467</v>
+        <v>486.68179515704668</v>
       </c>
       <c r="C94">
-        <v>0.0004963570979530794</v>
+        <v>4.9635709795307935E-4</v>
       </c>
       <c r="D94">
-        <v>0.03200487359035111</v>
+        <v>3.2004873590351111E-2</v>
       </c>
       <c r="E94">
-        <v>-3.134651645689342e-5</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
+        <v>-3.134651645689342E-5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>98</v>
       </c>
@@ -2555,33 +2560,33 @@
         <v>126.9767299474213</v>
       </c>
       <c r="C95">
-        <v>-0.0001655368056910255</v>
+        <v>-1.6553680569102549E-4</v>
       </c>
       <c r="D95">
-        <v>-0.024533559874365854</v>
+        <v>-2.4533559874365854E-2</v>
       </c>
       <c r="E95">
-        <v>2.4052914168587593e-5</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5">
+        <v>2.4052914168587593E-5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>99</v>
       </c>
       <c r="B96">
-        <v>84.70126745085186</v>
+        <v>84.701267450851859</v>
       </c>
       <c r="C96">
-        <v>0.00025591359885793034</v>
+        <v>2.5591359885793034E-4</v>
       </c>
       <c r="D96">
-        <v>0.02493392139591429</v>
+        <v>2.4933921395914289E-2</v>
       </c>
       <c r="E96">
-        <v>-2.4433808308527345e-5</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
+        <v>-2.4433808308527345E-5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>100</v>
       </c>
@@ -2589,50 +2594,50 @@
         <v>0.30066254435730366</v>
       </c>
       <c r="C97">
-        <v>-2.851398607942417e-6</v>
+        <v>-2.851398607942417E-6</v>
       </c>
       <c r="D97">
-        <v>-0.000310175485918379</v>
+        <v>-3.1017548591837898E-4</v>
       </c>
       <c r="E97">
-        <v>3.0613332341107063e-7</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
+        <v>3.0613332341107063E-7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>101</v>
       </c>
       <c r="B98">
-        <v>582.9335734881603</v>
+        <v>582.93357348816028</v>
       </c>
       <c r="C98">
-        <v>0.0031237528626846486</v>
+        <v>3.1237528626846486E-3</v>
       </c>
       <c r="D98">
-        <v>0.3178366623302741</v>
+        <v>0.31783666233027408</v>
       </c>
       <c r="E98">
-        <v>-0.00031196662490986447</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
+        <v>-3.1196662490986447E-4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>102</v>
       </c>
       <c r="B99">
-        <v>486.6817951570467</v>
+        <v>486.68179515704668</v>
       </c>
       <c r="C99">
-        <v>0.0004963570979530794</v>
+        <v>4.9635709795307935E-4</v>
       </c>
       <c r="D99">
-        <v>0.03200487359035111</v>
+        <v>3.2004873590351111E-2</v>
       </c>
       <c r="E99">
-        <v>-3.134651645689342e-5</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5">
+        <v>-3.134651645689342E-5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>103</v>
       </c>
@@ -2640,33 +2645,33 @@
         <v>126.9767299474213</v>
       </c>
       <c r="C100">
-        <v>-0.0001655368056910255</v>
+        <v>-1.6553680569102549E-4</v>
       </c>
       <c r="D100">
-        <v>-0.024533559874365854</v>
+        <v>-2.4533559874365854E-2</v>
       </c>
       <c r="E100">
-        <v>2.4052914168587593e-5</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5">
+        <v>2.4052914168587593E-5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>104</v>
       </c>
       <c r="B101">
-        <v>84.70126745085186</v>
+        <v>84.701267450851859</v>
       </c>
       <c r="C101">
-        <v>0.00025591359885793034</v>
+        <v>2.5591359885793034E-4</v>
       </c>
       <c r="D101">
-        <v>0.02493392139591429</v>
+        <v>2.4933921395914289E-2</v>
       </c>
       <c r="E101">
-        <v>-2.4433808308527345e-5</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5">
+        <v>-2.4433808308527345E-5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>105</v>
       </c>
@@ -2674,50 +2679,50 @@
         <v>0.30066254435730366</v>
       </c>
       <c r="C102">
-        <v>-2.851398607942417e-6</v>
+        <v>-2.851398607942417E-6</v>
       </c>
       <c r="D102">
-        <v>-0.000310175485918379</v>
+        <v>-3.1017548591837898E-4</v>
       </c>
       <c r="E102">
-        <v>3.0613332341107063e-7</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5">
+        <v>3.0613332341107063E-7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>106</v>
       </c>
       <c r="B103">
-        <v>582.9335734881603</v>
+        <v>582.93357348816028</v>
       </c>
       <c r="C103">
-        <v>0.0031237528626846486</v>
+        <v>3.1237528626846486E-3</v>
       </c>
       <c r="D103">
-        <v>0.3178366623302741</v>
+        <v>0.31783666233027408</v>
       </c>
       <c r="E103">
-        <v>-0.00031196662490986447</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5">
+        <v>-3.1196662490986447E-4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>107</v>
       </c>
       <c r="B104">
-        <v>486.6817951570467</v>
+        <v>486.68179515704668</v>
       </c>
       <c r="C104">
-        <v>0.0004963570979530794</v>
+        <v>4.9635709795307935E-4</v>
       </c>
       <c r="D104">
-        <v>0.03200487359035111</v>
+        <v>3.2004873590351111E-2</v>
       </c>
       <c r="E104">
-        <v>-3.134651645689342e-5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5">
+        <v>-3.134651645689342E-5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>108</v>
       </c>
@@ -2725,33 +2730,33 @@
         <v>126.9767299474213</v>
       </c>
       <c r="C105">
-        <v>-0.0001655368056910255</v>
+        <v>-1.6553680569102549E-4</v>
       </c>
       <c r="D105">
-        <v>-0.024533559874365854</v>
+        <v>-2.4533559874365854E-2</v>
       </c>
       <c r="E105">
-        <v>2.4052914168587593e-5</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5">
+        <v>2.4052914168587593E-5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>109</v>
       </c>
       <c r="B106">
-        <v>84.70126745085186</v>
+        <v>84.701267450851859</v>
       </c>
       <c r="C106">
-        <v>0.00025591359885793034</v>
+        <v>2.5591359885793034E-4</v>
       </c>
       <c r="D106">
-        <v>0.02493392139591429</v>
+        <v>2.4933921395914289E-2</v>
       </c>
       <c r="E106">
-        <v>-2.4433808308527345e-5</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5">
+        <v>-2.4433808308527345E-5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>110</v>
       </c>
@@ -2759,16 +2764,16 @@
         <v>0.30066254435730366</v>
       </c>
       <c r="C107">
-        <v>-2.851398607942417e-6</v>
+        <v>-2.851398607942417E-6</v>
       </c>
       <c r="D107">
-        <v>-0.000310175485918379</v>
+        <v>-3.1017548591837898E-4</v>
       </c>
       <c r="E107">
-        <v>3.0613332341107063e-7</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5">
+        <v>3.0613332341107063E-7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>111</v>
       </c>
@@ -2776,50 +2781,50 @@
         <v>464.63946108686514</v>
       </c>
       <c r="C108">
-        <v>0.0032401614565962665</v>
+        <v>3.2401614565962665E-3</v>
       </c>
       <c r="D108">
         <v>0.33653780018721086</v>
       </c>
       <c r="E108">
-        <v>-0.0003303037385328174</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5">
+        <v>-3.3030373853281742E-4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>112</v>
       </c>
       <c r="B109">
-        <v>604.9759075583419</v>
+        <v>604.97590755834187</v>
       </c>
       <c r="C109">
-        <v>0.0003799485040414098</v>
+        <v>3.7994850404140981E-4</v>
       </c>
       <c r="D109">
-        <v>0.013303613926337249</v>
+        <v>1.3303613926337249E-2</v>
       </c>
       <c r="E109">
-        <v>-1.3011101173552649e-5</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5">
+        <v>-1.3011101173552649E-5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>113</v>
       </c>
       <c r="B110">
-        <v>8.682617546126195</v>
+        <v>8.6826175461261954</v>
       </c>
       <c r="C110">
-        <v>-4.9128209336013694e-5</v>
+        <v>-4.9128209336013694E-5</v>
       </c>
       <c r="D110">
-        <v>-0.005832409328972993</v>
+        <v>-5.8324093289729931E-3</v>
       </c>
       <c r="E110">
-        <v>5.716543568921671e-6</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5">
+        <v>5.7165435689216708E-6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>114</v>
       </c>
@@ -2827,16 +2832,16 @@
         <v>202.99537985214695</v>
       </c>
       <c r="C111">
-        <v>0.00013950501471996226</v>
+        <v>1.3950501471996226E-4</v>
       </c>
       <c r="D111">
-        <v>0.006232793689309271</v>
+        <v>6.2327936893092706E-3</v>
       </c>
       <c r="E111">
-        <v>-6.097119270145444e-6</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5">
+        <v>-6.0971192701454443E-6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>115</v>
       </c>
@@ -2844,16 +2849,16 @@
         <v>0.30066254435730366</v>
       </c>
       <c r="C112">
-        <v>-2.851398607942417e-6</v>
+        <v>-2.851398607942417E-6</v>
       </c>
       <c r="D112">
-        <v>-0.000310175485918379</v>
+        <v>-3.1017548591837898E-4</v>
       </c>
       <c r="E112">
-        <v>3.0613332341107063e-7</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5">
+        <v>3.0613332341107063E-7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>116</v>
       </c>
@@ -2861,50 +2866,50 @@
         <v>464.63946108686514</v>
       </c>
       <c r="C113">
-        <v>0.0032401614565962665</v>
+        <v>3.2401614565962665E-3</v>
       </c>
       <c r="D113">
         <v>0.33653780018721086</v>
       </c>
       <c r="E113">
-        <v>-0.0003303037385328174</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5">
+        <v>-3.3030373853281742E-4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>117</v>
       </c>
       <c r="B114">
-        <v>604.9759075583419</v>
+        <v>604.97590755834187</v>
       </c>
       <c r="C114">
-        <v>0.0003799485040414098</v>
+        <v>3.7994850404140981E-4</v>
       </c>
       <c r="D114">
-        <v>0.013303613926337249</v>
+        <v>1.3303613926337249E-2</v>
       </c>
       <c r="E114">
-        <v>-1.3011101173552649e-5</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5">
+        <v>-1.3011101173552649E-5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>118</v>
       </c>
       <c r="B115">
-        <v>8.682617546126195</v>
+        <v>8.6826175461261954</v>
       </c>
       <c r="C115">
-        <v>-4.9128209336013694e-5</v>
+        <v>-4.9128209336013694E-5</v>
       </c>
       <c r="D115">
-        <v>-0.005832409328972993</v>
+        <v>-5.8324093289729931E-3</v>
       </c>
       <c r="E115">
-        <v>5.716543568921671e-6</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5">
+        <v>5.7165435689216708E-6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>119</v>
       </c>
@@ -2912,16 +2917,16 @@
         <v>202.99537985214695</v>
       </c>
       <c r="C116">
-        <v>0.00013950501471996226</v>
+        <v>1.3950501471996226E-4</v>
       </c>
       <c r="D116">
-        <v>0.006232793689309271</v>
+        <v>6.2327936893092706E-3</v>
       </c>
       <c r="E116">
-        <v>-6.097119270145444e-6</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5">
+        <v>-6.0971192701454443E-6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>120</v>
       </c>
@@ -2929,16 +2934,16 @@
         <v>0.30066254435730366</v>
       </c>
       <c r="C117">
-        <v>-2.851398607942417e-6</v>
+        <v>-2.851398607942417E-6</v>
       </c>
       <c r="D117">
-        <v>-0.000310175485918379</v>
+        <v>-3.1017548591837898E-4</v>
       </c>
       <c r="E117">
-        <v>3.0613332341107063e-7</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5">
+        <v>3.0613332341107063E-7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>121</v>
       </c>
@@ -2946,50 +2951,50 @@
         <v>464.63946108686514</v>
       </c>
       <c r="C118">
-        <v>0.0032401614565962665</v>
+        <v>3.2401614565962665E-3</v>
       </c>
       <c r="D118">
         <v>0.33653780018721086</v>
       </c>
       <c r="E118">
-        <v>-0.0003303037385328174</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5">
+        <v>-3.3030373853281742E-4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>122</v>
       </c>
       <c r="B119">
-        <v>604.9759075583419</v>
+        <v>604.97590755834187</v>
       </c>
       <c r="C119">
-        <v>0.0003799485040414098</v>
+        <v>3.7994850404140981E-4</v>
       </c>
       <c r="D119">
-        <v>0.013303613926337249</v>
+        <v>1.3303613926337249E-2</v>
       </c>
       <c r="E119">
-        <v>-1.3011101173552649e-5</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5">
+        <v>-1.3011101173552649E-5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>123</v>
       </c>
       <c r="B120">
-        <v>8.682617546126195</v>
+        <v>8.6826175461261954</v>
       </c>
       <c r="C120">
-        <v>-4.9128209336013694e-5</v>
+        <v>-4.9128209336013694E-5</v>
       </c>
       <c r="D120">
-        <v>-0.005832409328972993</v>
+        <v>-5.8324093289729931E-3</v>
       </c>
       <c r="E120">
-        <v>5.716543568921671e-6</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5">
+        <v>5.7165435689216708E-6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>124</v>
       </c>
@@ -2997,16 +3002,16 @@
         <v>202.99537985214695</v>
       </c>
       <c r="C121">
-        <v>0.00013950501471996226</v>
+        <v>1.3950501471996226E-4</v>
       </c>
       <c r="D121">
-        <v>0.006232793689309271</v>
+        <v>6.2327936893092706E-3</v>
       </c>
       <c r="E121">
-        <v>-6.097119270145444e-6</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5">
+        <v>-6.0971192701454443E-6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>125</v>
       </c>
@@ -3014,16 +3019,16 @@
         <v>0.30066254435730366</v>
       </c>
       <c r="C122">
-        <v>-2.851398607942417e-6</v>
+        <v>-2.851398607942417E-6</v>
       </c>
       <c r="D122">
-        <v>-0.000310175485918379</v>
+        <v>-3.1017548591837898E-4</v>
       </c>
       <c r="E122">
-        <v>3.0613332341107063e-7</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5">
+        <v>3.0613332341107063E-7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>126</v>
       </c>
@@ -3031,50 +3036,50 @@
         <v>464.63946108686514</v>
       </c>
       <c r="C123">
-        <v>0.0032401614565962665</v>
+        <v>3.2401614565962665E-3</v>
       </c>
       <c r="D123">
         <v>0.33653780018721086</v>
       </c>
       <c r="E123">
-        <v>-0.0003303037385328174</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5">
+        <v>-3.3030373853281742E-4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>127</v>
       </c>
       <c r="B124">
-        <v>604.9759075583419</v>
+        <v>604.97590755834187</v>
       </c>
       <c r="C124">
-        <v>0.0003799485040414098</v>
+        <v>3.7994850404140981E-4</v>
       </c>
       <c r="D124">
-        <v>0.013303613926337249</v>
+        <v>1.3303613926337249E-2</v>
       </c>
       <c r="E124">
-        <v>-1.3011101173552649e-5</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5">
+        <v>-1.3011101173552649E-5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>128</v>
       </c>
       <c r="B125">
-        <v>8.682617546126195</v>
+        <v>8.6826175461261954</v>
       </c>
       <c r="C125">
-        <v>-4.9128209336013694e-5</v>
+        <v>-4.9128209336013694E-5</v>
       </c>
       <c r="D125">
-        <v>-0.005832409328972993</v>
+        <v>-5.8324093289729931E-3</v>
       </c>
       <c r="E125">
-        <v>5.716543568921671e-6</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5">
+        <v>5.7165435689216708E-6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>129</v>
       </c>
@@ -3082,16 +3087,16 @@
         <v>202.99537985214695</v>
       </c>
       <c r="C126">
-        <v>0.00013950501471996226</v>
+        <v>1.3950501471996226E-4</v>
       </c>
       <c r="D126">
-        <v>0.006232793689309271</v>
+        <v>6.2327936893092706E-3</v>
       </c>
       <c r="E126">
-        <v>-6.097119270145444e-6</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5">
+        <v>-6.0971192701454443E-6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>130</v>
       </c>
@@ -3099,186 +3104,186 @@
         <v>463.34597144451664</v>
       </c>
       <c r="C127">
-        <v>0.0032394243375312194</v>
+        <v>3.2394243375312194E-3</v>
       </c>
       <c r="D127">
-        <v>0.3365168047724011</v>
+        <v>0.33651680477240109</v>
       </c>
       <c r="E127">
-        <v>-0.0003302917845126979</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5">
+        <v>-3.3029178451269789E-4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>131</v>
       </c>
       <c r="B128">
-        <v>3.6744648701291255e-10</v>
+        <v>3.6744648701291255E-10</v>
       </c>
       <c r="C128">
-        <v>-3.695017194905453e-15</v>
+        <v>-3.695017194905453E-15</v>
       </c>
       <c r="D128">
-        <v>-3.850984010421278e-13</v>
+        <v>-3.850984010421278E-13</v>
       </c>
       <c r="E128">
-        <v>3.8002002270167146e-16</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5">
+        <v>3.8002002270167146E-16</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>132</v>
       </c>
       <c r="B129">
-        <v>0.999999001581369</v>
+        <v>0.99999900158136901</v>
       </c>
       <c r="C129">
-        <v>1.5271297772596267e-13</v>
+        <v>1.5271297772596267E-13</v>
       </c>
       <c r="D129">
-        <v>2.379040710097595e-10</v>
+        <v>2.379040710097595E-10</v>
       </c>
       <c r="E129">
-        <v>6.634139022464255e-12</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5">
+        <v>6.6341390224642549E-12</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>133</v>
       </c>
       <c r="B130">
-        <v>7.393547222017354e-7</v>
+        <v>7.3935472220173544E-7</v>
       </c>
       <c r="C130">
-        <v>4.1273665806713616e-14</v>
+        <v>4.1273665806713616E-14</v>
       </c>
       <c r="D130">
-        <v>4.137194055607425e-12</v>
+        <v>4.1371940556074246E-12</v>
       </c>
       <c r="E130">
-        <v>-4.053631555099665e-15</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5">
+        <v>-4.0536315550996648E-15</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>134</v>
       </c>
       <c r="B131">
-        <v>1.0611223031523729e-8</v>
+        <v>1.0611223031523729E-8</v>
       </c>
       <c r="C131">
-        <v>-6.611259630082474e-14</v>
+        <v>-6.6112596300824743E-14</v>
       </c>
       <c r="D131">
-        <v>-7.301919843523602e-12</v>
+        <v>-7.3019198435236023E-12</v>
       </c>
       <c r="E131">
-        <v>7.156332774549773e-15</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5">
+        <v>7.156332774549773E-15</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>135</v>
       </c>
       <c r="B132">
-        <v>2.4808523910408143e-7</v>
+        <v>2.4808523910408143E-7</v>
       </c>
       <c r="C132">
-        <v>2.8534073273718374e-14</v>
+        <v>2.8534073273718374E-14</v>
       </c>
       <c r="D132">
-        <v>3.5499059843691758e-12</v>
+        <v>3.5499059843691758E-12</v>
       </c>
       <c r="E132">
-        <v>-3.4784009107192957e-15</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5">
+        <v>-3.4784009107192957E-15</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>136</v>
       </c>
       <c r="B133">
-        <v>818.2480571433209</v>
+        <v>818.24805714332092</v>
       </c>
       <c r="C133">
-        <v>0.0004682109325660711</v>
+        <v>4.6821093256607112E-4</v>
       </c>
       <c r="D133">
-        <v>0.013414677732467266</v>
+        <v>1.3414677732467266E-2</v>
       </c>
       <c r="E133">
-        <v>-1.3107103803341968e-5</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5">
+        <v>-1.3107103803341968E-5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>137</v>
       </c>
       <c r="B134">
-        <v>0.00036744648701291253</v>
+        <v>3.6744648701291253E-4</v>
       </c>
       <c r="C134">
-        <v>-3.6950171706111338e-9</v>
+        <v>-3.6950171706111338E-9</v>
       </c>
       <c r="D134">
-        <v>-3.850983775950526e-7</v>
+        <v>-3.8509837759505263E-7</v>
       </c>
       <c r="E134">
-        <v>3.800194353959724e-10</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5">
+        <v>3.8001943539597241E-10</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>138</v>
       </c>
       <c r="B135">
-        <v>0.0015813691756464694</v>
+        <v>1.5813691756464694E-3</v>
       </c>
       <c r="C135">
-        <v>-5.1003735079343927e-14</v>
+        <v>-5.1003735079343927E-14</v>
       </c>
       <c r="D135">
-        <v>-2.4162232769585173e-11</v>
+        <v>-2.4162232769585173E-11</v>
       </c>
       <c r="E135">
-        <v>1.2957313907837354e-14</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5">
+        <v>1.2957313907837354E-14</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>139</v>
       </c>
       <c r="B136">
-        <v>0.7393547222017355</v>
+        <v>0.73935472220173548</v>
       </c>
       <c r="C136">
-        <v>4.127364481145475e-8</v>
+        <v>4.1273644811454753E-8</v>
       </c>
       <c r="D136">
-        <v>4.137208750795445e-6</v>
+        <v>4.137208750795445E-6</v>
       </c>
       <c r="E136">
-        <v>-4.053170558985474e-9</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5">
+        <v>-4.0531705589854741E-9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>140</v>
       </c>
       <c r="B137">
-        <v>0.01061122303152373</v>
+        <v>1.0611223031523729E-2</v>
       </c>
       <c r="C137">
-        <v>-6.611259666776075e-8</v>
+        <v>-6.6112596667760748E-8</v>
       </c>
       <c r="D137">
-        <v>-7.301919061602361e-6</v>
+        <v>-7.3019190616023606E-6</v>
       </c>
       <c r="E137">
-        <v>7.156348259406545e-9</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5">
+        <v>7.1563482594065448E-9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>141</v>
       </c>
@@ -3286,16 +3291,16 @@
         <v>0.2480852391040814</v>
       </c>
       <c r="C138">
-        <v>2.8534106118092086e-8</v>
+        <v>2.8534106118092086E-8</v>
       </c>
       <c r="D138">
-        <v>3.549911494692277e-6</v>
+        <v>3.5499114946922771E-6</v>
       </c>
       <c r="E138">
-        <v>-3.4772643122346917e-9</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5">
+        <v>-3.4772643122346917E-9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>142</v>
       </c>
@@ -3303,16 +3308,16 @@
         <v>0.30066237410245417</v>
       </c>
       <c r="C139">
-        <v>-2.85139809478208e-6</v>
+        <v>-2.8513980947820799E-6</v>
       </c>
       <c r="D139">
-        <v>-0.00031017543117581173</v>
+        <v>-3.1017543117581173E-4</v>
       </c>
       <c r="E139">
-        <v>3.0613326870359305e-7</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5">
+        <v>3.0613326870359305E-7</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>143</v>
       </c>
@@ -3320,50 +3325,50 @@
         <v>1.2939522555990586</v>
       </c>
       <c r="C140">
-        <v>7.403725391180017e-7</v>
+        <v>7.403725391180017E-7</v>
       </c>
       <c r="D140">
-        <v>2.119371666607169e-5</v>
+        <v>2.119371666607169E-5</v>
       </c>
       <c r="E140">
-        <v>-2.0722439448492282e-8</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5">
+        <v>-2.0722439448492282E-8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>144</v>
       </c>
       <c r="B141">
-        <v>604.9755649813098</v>
+        <v>604.97556498130984</v>
       </c>
       <c r="C141">
-        <v>0.00037994607829758335</v>
+        <v>3.7994607829758335E-4</v>
       </c>
       <c r="D141">
-        <v>0.013303525625987318</v>
+        <v>1.3303525625987318E-2</v>
       </c>
       <c r="E141">
-        <v>-1.3010855069565421e-5</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5">
+        <v>-1.3010855069565421E-5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>145</v>
       </c>
       <c r="B142">
-        <v>8.682612629458752</v>
+        <v>8.6826126294587525</v>
       </c>
       <c r="C142">
-        <v>-4.912821299983866e-5</v>
+        <v>-4.9128212999838661E-5</v>
       </c>
       <c r="D142">
-        <v>-0.005832410785979175</v>
+        <v>-5.8324107859791747E-3</v>
       </c>
       <c r="E142">
-        <v>5.716490680388389e-6</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5">
+        <v>5.7164906803883886E-6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>146</v>
       </c>
@@ -3371,84 +3376,84 @@
         <v>202.99526490285083</v>
       </c>
       <c r="C143">
-        <v>0.00013950419308003082</v>
+        <v>1.3950419308003082E-4</v>
       </c>
       <c r="D143">
-        <v>0.006232688262625831</v>
+        <v>6.2326882626258309E-3</v>
       </c>
       <c r="E143">
-        <v>-6.097884878601087e-6</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5">
+        <v>-6.0978848786010869E-6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>147</v>
       </c>
       <c r="B144">
-        <v>0.0003006623741024542</v>
+        <v>3.0066237410245419E-4</v>
       </c>
       <c r="C144">
-        <v>-2.8513981079058764e-9</v>
+        <v>-2.8513981079058764E-9</v>
       </c>
       <c r="D144">
-        <v>-3.10175444186151e-7</v>
+        <v>-3.1017544418615098E-7</v>
       </c>
       <c r="E144">
-        <v>3.0613289294177666e-10</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5">
+        <v>3.0613289294177666E-10</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>148</v>
       </c>
       <c r="B145">
-        <v>0.0012939522555990585</v>
+        <v>1.2939522555990585E-3</v>
       </c>
       <c r="C145">
-        <v>7.403725737171084e-10</v>
+        <v>7.4037257371710842E-10</v>
       </c>
       <c r="D145">
-        <v>2.1193778619659082e-8</v>
+        <v>2.1193778619659082E-8</v>
       </c>
       <c r="E145">
-        <v>-2.0717204698031633e-11</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5">
+        <v>-2.0717204698031633E-11</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>149</v>
       </c>
       <c r="B146">
-        <v>586.8262980318706</v>
+        <v>586.82629803187058</v>
       </c>
       <c r="C146">
-        <v>0.000368547652944693</v>
+        <v>3.6854765294469299E-4</v>
       </c>
       <c r="D146">
-        <v>0.012904404428447367</v>
+        <v>1.2904404428447367E-2</v>
       </c>
       <c r="E146">
-        <v>-1.2623110893488749e-5</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5">
+        <v>-1.2623110893488749E-5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>150</v>
       </c>
       <c r="B147">
-        <v>0.008682612629458753</v>
+        <v>8.6826126294587535E-3</v>
       </c>
       <c r="C147">
-        <v>-4.912821412609745e-8</v>
+        <v>-4.9128214126097448E-8</v>
       </c>
       <c r="D147">
-        <v>-5.832410300254908e-6</v>
+        <v>-5.8324103002549077E-6</v>
       </c>
       <c r="E147">
-        <v>5.716444241419555e-9</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5">
+        <v>5.7164442414195553E-9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>151</v>
       </c>
@@ -3456,33 +3461,33 @@
         <v>0.20299526490285083</v>
       </c>
       <c r="C148">
-        <v>1.3950420835132755e-7</v>
+        <v>1.3950420835132755E-7</v>
       </c>
       <c r="D148">
-        <v>6.2326909588743625e-6</v>
+        <v>6.2326909588743625E-6</v>
       </c>
       <c r="E148">
-        <v>-6.097354147540298e-9</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5">
+        <v>-6.0973541475402977E-9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>152</v>
       </c>
       <c r="B149">
-        <v>0.3003617117283517</v>
+        <v>0.30036171172835169</v>
       </c>
       <c r="C149">
-        <v>-2.848546692945845e-6</v>
+        <v>-2.8485466929458452E-6</v>
       </c>
       <c r="D149">
-        <v>-0.00030986523040786834</v>
+        <v>-3.0986523040786834E-4</v>
       </c>
       <c r="E149">
-        <v>3.0582708236189036e-7</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5">
+        <v>3.0582708236189036E-7</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>153</v>
       </c>
@@ -3490,16 +3495,16 @@
         <v>1.2926583033434595</v>
       </c>
       <c r="C150">
-        <v>7.396321714657109e-7</v>
+        <v>7.3963217146571089E-7</v>
       </c>
       <c r="D150">
-        <v>2.1172507089065867e-5</v>
+        <v>2.1172507089065867E-5</v>
       </c>
       <c r="E150">
-        <v>-2.0701663935929357e-8</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5">
+        <v>-2.0701663935929357E-8</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>154</v>
       </c>
@@ -3507,33 +3512,33 @@
         <v>18.149266949439312</v>
       </c>
       <c r="C151">
-        <v>1.1398381371564244e-5</v>
+        <v>1.1398381371564244E-5</v>
       </c>
       <c r="D151">
-        <v>0.00039910597179003155</v>
+        <v>3.9910597179003155E-4</v>
       </c>
       <c r="E151">
-        <v>-3.902916852976522e-7</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5">
+        <v>-3.902916852976522E-7</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>155</v>
       </c>
       <c r="B152">
-        <v>8.673930016829294</v>
+        <v>8.6739300168292939</v>
       </c>
       <c r="C152">
-        <v>-4.907908499330655e-5</v>
+        <v>-4.9079084993306551E-5</v>
       </c>
       <c r="D152">
-        <v>-0.0058265786073877415</v>
+        <v>-5.8265786073877415E-3</v>
       </c>
       <c r="E152">
-        <v>5.710765114206288e-6</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5">
+        <v>5.710765114206288E-6</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>156</v>
       </c>
@@ -3541,33 +3546,33 @@
         <v>202.79226963794798</v>
       </c>
       <c r="C153">
-        <v>0.00013936469230772596</v>
+        <v>1.3936469230772596E-4</v>
       </c>
       <c r="D153">
-        <v>0.006226456305185589</v>
+        <v>6.2264563051855886E-3</v>
       </c>
       <c r="E153">
-        <v>-6.091774256156816e-6</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5">
+        <v>-6.0917742561568159E-6</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>157</v>
       </c>
       <c r="B154">
-        <v>311.0</v>
+        <v>311</v>
       </c>
       <c r="C154">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D154">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E154">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>158</v>
       </c>
@@ -3575,33 +3580,33 @@
         <v>397.24612753336663</v>
       </c>
       <c r="C155">
-        <v>8.654770716481508e-5</v>
+        <v>8.6547707164815079E-5</v>
       </c>
       <c r="D155">
-        <v>0.009515130347816956</v>
+        <v>9.5151303478169559E-3</v>
       </c>
       <c r="E155">
-        <v>-9.371370374044987e-6</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5">
+        <v>-9.3713703740449868E-6</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>159</v>
       </c>
       <c r="B156">
-        <v>423.0</v>
+        <v>423</v>
       </c>
       <c r="C156">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D156">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E156">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>160</v>
       </c>
@@ -3609,118 +3614,118 @@
         <v>397.24612753336663</v>
       </c>
       <c r="C157">
-        <v>8.654770716481508e-5</v>
+        <v>8.6547707164815079E-5</v>
       </c>
       <c r="D157">
-        <v>0.009515130347816956</v>
+        <v>9.5151303478169559E-3</v>
       </c>
       <c r="E157">
-        <v>-9.371370374044987e-6</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5">
+        <v>-9.3713703740449868E-6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>161</v>
       </c>
       <c r="B158">
-        <v>644.5953165006283</v>
+        <v>644.59531650062831</v>
       </c>
       <c r="C158">
-        <v>2.6654204647555803e-7</v>
+        <v>2.6654204647555803E-7</v>
       </c>
       <c r="D158">
-        <v>-0.0004903608496892539</v>
+        <v>-4.9036084968925387E-4</v>
       </c>
       <c r="E158">
-        <v>2.586573388751261e-7</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5">
+        <v>2.5865733887512611E-7</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>162</v>
       </c>
       <c r="B159">
-        <v>609.2000001706484</v>
+        <v>609.20000017064842</v>
       </c>
       <c r="C159">
-        <v>-9.203628341727306e-5</v>
+        <v>-9.203628341727306E-5</v>
       </c>
       <c r="D159">
-        <v>-0.010474326311733013</v>
+        <v>-1.0474326311733013E-2</v>
       </c>
       <c r="E159">
-        <v>1.0129740100090409e-5</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5">
+        <v>1.0129740100090409E-5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>163</v>
       </c>
       <c r="B160">
-        <v>609.2000003471878</v>
+        <v>609.20000034718782</v>
       </c>
       <c r="C160">
-        <v>-0.00011261939985296618</v>
+        <v>-1.1261939985296618E-4</v>
       </c>
       <c r="D160">
-        <v>-0.0104747898276758</v>
+        <v>-1.0474789827675799E-2</v>
       </c>
       <c r="E160">
-        <v>1.0075449927550787e-5</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5">
+        <v>1.0075449927550787E-5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>164</v>
       </c>
       <c r="B161">
-        <v>609.2000003471878</v>
+        <v>609.20000034718782</v>
       </c>
       <c r="C161">
-        <v>-0.00011261939985296618</v>
+        <v>-1.1261939985296618E-4</v>
       </c>
       <c r="D161">
-        <v>-0.0104747898276758</v>
+        <v>-1.0474789827675799E-2</v>
       </c>
       <c r="E161">
-        <v>1.0075449927550787e-5</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5">
+        <v>1.0075449927550787E-5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>165</v>
       </c>
       <c r="B162">
-        <v>951.4824081015402</v>
+        <v>951.48240810154016</v>
       </c>
       <c r="C162">
-        <v>2.9550040167310714e-5</v>
+        <v>2.9550040167310714E-5</v>
       </c>
       <c r="D162">
-        <v>-0.00028899458167839365</v>
+        <v>-2.8899458167839365E-4</v>
       </c>
       <c r="E162">
-        <v>1.6475887447553207e-7</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5">
+        <v>1.6475887447553207E-7</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>166</v>
       </c>
       <c r="B163">
-        <v>951.4824081015402</v>
+        <v>951.48240810154016</v>
       </c>
       <c r="C163">
-        <v>2.9550040167310714e-5</v>
+        <v>2.9550040167310714E-5</v>
       </c>
       <c r="D163">
-        <v>-0.00028899458167839365</v>
+        <v>-2.8899458167839365E-4</v>
       </c>
       <c r="E163">
-        <v>1.6475887447553207e-7</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5">
+        <v>1.6475887447553207E-7</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>167</v>
       </c>
@@ -3728,33 +3733,33 @@
         <v>1291.817465833818</v>
       </c>
       <c r="C164">
-        <v>5.573264255045872e-6</v>
+        <v>5.573264255045872E-6</v>
       </c>
       <c r="D164">
-        <v>-0.0032743778048596466</v>
+        <v>-3.2743778048596466E-3</v>
       </c>
       <c r="E164">
-        <v>2.8822564879528025e-6</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5">
+        <v>2.8822564879528025E-6</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>168</v>
       </c>
       <c r="B165">
-        <v>634.2000005057195</v>
+        <v>634.20000050571946</v>
       </c>
       <c r="C165">
-        <v>-0.0001759809289216692</v>
+        <v>-1.7598092892166919E-4</v>
       </c>
       <c r="D165">
-        <v>-0.010475709676457223</v>
+        <v>-1.0475709676457223E-2</v>
       </c>
       <c r="E165">
-        <v>1.0052333800568356e-5</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5">
+        <v>1.0052333800568356E-5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>169</v>
       </c>
@@ -3762,16 +3767,16 @@
         <v>293.00000003068044</v>
       </c>
       <c r="C166">
-        <v>-5.864176881497936e-10</v>
+        <v>-5.8641768814979361E-10</v>
       </c>
       <c r="D166">
-        <v>-2.8421707989590313e-7</v>
+        <v>-2.8421707989590313E-7</v>
       </c>
       <c r="E166">
-        <v>-1.268269837976284e-17</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5">
+        <v>-1.268269837976284E-17</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>170</v>
       </c>
@@ -3779,16 +3784,16 @@
         <v>293.00000003068044</v>
       </c>
       <c r="C167">
-        <v>-5.864176881497936e-10</v>
+        <v>-5.8641768814979361E-10</v>
       </c>
       <c r="D167">
-        <v>-2.8421707989590313e-7</v>
+        <v>-2.8421707989590313E-7</v>
       </c>
       <c r="E167">
-        <v>-1.268269837976284e-17</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5">
+        <v>-1.268269837976284E-17</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>171</v>
       </c>
@@ -3796,16 +3801,16 @@
         <v>293.00000003068044</v>
       </c>
       <c r="C168">
-        <v>-5.864176881497936e-10</v>
+        <v>-5.8641768814979361E-10</v>
       </c>
       <c r="D168">
-        <v>-2.8421707989590313e-7</v>
+        <v>-2.8421707989590313E-7</v>
       </c>
       <c r="E168">
-        <v>-1.268269837976284e-17</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5">
+        <v>-1.268269837976284E-17</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>172</v>
       </c>
@@ -3813,16 +3818,16 @@
         <v>293.00000003068044</v>
       </c>
       <c r="C169">
-        <v>-5.864176881497936e-10</v>
+        <v>-5.8641768814979361E-10</v>
       </c>
       <c r="D169">
-        <v>-2.8421707989590313e-7</v>
+        <v>-2.8421707989590313E-7</v>
       </c>
       <c r="E169">
-        <v>-1.268269837976284e-17</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5">
+        <v>-1.268269837976284E-17</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>173</v>
       </c>
@@ -3830,16 +3835,16 @@
         <v>293.00000003068044</v>
       </c>
       <c r="C170">
-        <v>-5.864176881497936e-10</v>
+        <v>-5.8641768814979361E-10</v>
       </c>
       <c r="D170">
-        <v>-2.8421707989590313e-7</v>
+        <v>-2.8421707989590313E-7</v>
       </c>
       <c r="E170">
-        <v>-1.268269837976284e-17</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5">
+        <v>-1.268269837976284E-17</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>174</v>
       </c>
@@ -3847,16 +3852,16 @@
         <v>293.00000003068044</v>
       </c>
       <c r="C171">
-        <v>-5.864176881497936e-10</v>
+        <v>-5.8641768814979361E-10</v>
       </c>
       <c r="D171">
-        <v>-2.8421707989590313e-7</v>
+        <v>-2.8421707989590313E-7</v>
       </c>
       <c r="E171">
-        <v>-1.268269837976284e-17</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5">
+        <v>-1.268269837976284E-17</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>175</v>
       </c>
@@ -3864,21 +3869,21 @@
         <v>293.00000003068044</v>
       </c>
       <c r="C172">
-        <v>-5.864176881497936e-10</v>
+        <v>-5.8641768814979361E-10</v>
       </c>
       <c r="D172">
-        <v>-2.8421707989590313e-7</v>
+        <v>-2.8421707989590313E-7</v>
       </c>
       <c r="E172">
-        <v>-1.268269837976284e-17</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5">
+        <v>-1.268269837976284E-17</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>176</v>
       </c>
       <c r="B173">
-        <v>8.520619788545916e6</v>
+        <v>8520619.7885459159</v>
       </c>
       <c r="C173">
         <v>28.333624069470776</v>
@@ -3890,126 +3895,126 @@
         <v>-2.6692718576378596</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>177</v>
       </c>
       <c r="B174">
-        <v>0.006445518851880394</v>
+        <v>6.4455188518803943E-3</v>
       </c>
       <c r="C174">
-        <v>-0.7515139137307857</v>
+        <v>-0.75151391373078569</v>
       </c>
       <c r="D174">
-        <v>-0.003953266579467651</v>
+        <v>-3.9532665794676514E-3</v>
       </c>
       <c r="E174">
-        <v>-0.0017476453405266836</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5">
+        <v>-1.7476453405266836E-3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>178</v>
       </c>
       <c r="B175">
-        <v>3.0741855963244434e7</v>
+        <v>30741855.963244434</v>
       </c>
       <c r="C175">
         <v>105.68875347588651</v>
       </c>
       <c r="D175">
-        <v>9666.849578047071</v>
+        <v>9666.8495780470712</v>
       </c>
       <c r="E175">
-        <v>-9.494044265839591</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5">
+        <v>-9.4940442658395909</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>179</v>
       </c>
       <c r="B176">
-        <v>-3.0741855963244434e7</v>
+        <v>-30741855.963244434</v>
       </c>
       <c r="C176">
         <v>-105.68875347588651</v>
       </c>
       <c r="D176">
-        <v>-9666.849578047071</v>
+        <v>-9666.8495780470712</v>
       </c>
       <c r="E176">
-        <v>9.494044265839591</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5">
+        <v>9.4940442658395909</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>180</v>
       </c>
       <c r="B177">
-        <v>-1.1511342642409405e7</v>
+        <v>-11511342.642409405</v>
       </c>
       <c r="C177">
-        <v>-9.133483493501302</v>
+        <v>-9.1334834935013021</v>
       </c>
       <c r="D177">
-        <v>-852.2343336192714</v>
+        <v>-852.23433361927141</v>
       </c>
       <c r="E177">
-        <v>0.8394892095721057</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5">
+        <v>0.83948920957210571</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>181</v>
       </c>
       <c r="B178">
-        <v>-7.658230168887455e6</v>
+        <v>-7658230.168887455</v>
       </c>
       <c r="C178">
         <v>-22.357280238825265</v>
       </c>
       <c r="D178">
-        <v>-2114.539589680711</v>
+        <v>-2114.5395896807108</v>
       </c>
       <c r="E178">
-        <v>2.081586940532851</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5">
+        <v>2.0815869405328509</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>182</v>
       </c>
       <c r="B179">
-        <v>716.8219938295638</v>
+        <v>716.82199382956378</v>
       </c>
       <c r="C179">
-        <v>0.0034684914754603167</v>
+        <v>3.4684914754603167E-3</v>
       </c>
       <c r="D179">
         <v>0.34907069314935024</v>
       </c>
       <c r="E179">
-        <v>-0.00034258103152575114</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5">
+        <v>-3.4258103152575114E-4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>183</v>
       </c>
       <c r="B180">
-        <v>556.9992134084249</v>
+        <v>556.99921340842491</v>
       </c>
       <c r="C180">
-        <v>4.132012278528334</v>
+        <v>4.1320122785283342</v>
       </c>
       <c r="D180">
-        <v>0.0031534872749622903</v>
+        <v>3.1534872749622903E-3</v>
       </c>
       <c r="E180">
-        <v>-3.06106540322655e-6</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5">
+        <v>-3.0610654032265502E-6</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>184</v>
       </c>
@@ -4017,16 +4022,16 @@
         <v>29.827084623445646</v>
       </c>
       <c r="C181">
-        <v>-4.131643730828965</v>
+        <v>-4.1316437308289649</v>
       </c>
       <c r="D181">
-        <v>0.009750909540247573</v>
+        <v>9.7509095402475727E-3</v>
       </c>
       <c r="E181">
-        <v>-9.561833197568391e-6</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5">
+        <v>-9.561833197568391E-6</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>185</v>
       </c>
@@ -4034,50 +4039,50 @@
         <v>145.39999996064918</v>
       </c>
       <c r="C182">
-        <v>6.0035248187718326e-5</v>
+        <v>6.0035248187718326E-5</v>
       </c>
       <c r="D182">
-        <v>6.187401141401861e-5</v>
+        <v>6.1874011414018613E-5</v>
       </c>
       <c r="E182">
-        <v>-5.075901909500614e-8</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5">
+        <v>-5.0759019095006141E-8</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>186</v>
       </c>
       <c r="B183">
-        <v>3.9350816723423464e-8</v>
+        <v>3.9350816723423464E-8</v>
       </c>
       <c r="C183">
-        <v>0.9999399647447446</v>
+        <v>0.99993996474474456</v>
       </c>
       <c r="D183">
-        <v>-6.18625596611046e-5</v>
+        <v>-6.1862559661104595E-5</v>
       </c>
       <c r="E183">
-        <v>5.1225662122239735e-8</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5">
+        <v>5.1225662122239735E-8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>187</v>
       </c>
       <c r="B184">
-        <v>1.3897313754221703e-7</v>
+        <v>1.3897313754221703E-7</v>
       </c>
       <c r="C184">
-        <v>3.531433546377009</v>
+        <v>3.5314335463770088</v>
       </c>
       <c r="D184">
-        <v>-0.00021847663475251352</v>
+        <v>-2.1847663475251352E-4</v>
       </c>
       <c r="E184">
-        <v>1.8091088268521238e-7</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5">
+        <v>1.8091088268521238E-7</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>188</v>
       </c>
@@ -4088,10 +4093,10 @@
         <v>3.5315331214501007</v>
       </c>
       <c r="D185">
-        <v>0.0002918085800825295</v>
+        <v>2.9180858008252949E-4</v>
       </c>
       <c r="E185">
-        <v>-3.053720802971955e-7</v>
+        <v>-3.053720802971955E-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a bug where disturbance change did not work
</commit_message>
<xml_diff>
--- a/data/F.xlsx
+++ b/data/F.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\songc\Documents\NTNU\Emner\5. året\TKP4900 Master\JuMP Model\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/tmp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044CC9EE-277A-4821-A5C2-23B89B51CC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="189">
   <si>
     <t>Variable</t>
   </si>
@@ -647,7 +647,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -945,16 +945,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="G178" sqref="G178"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="21.59765625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -971,7 +966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -979,67 +974,67 @@
         <v>113.76095996921192</v>
       </c>
       <c r="C2">
-        <v>4.6971578963950364E-5</v>
+        <v>4.6971578963950364e-5</v>
       </c>
       <c r="D2">
-        <v>4.8404119892650542E-5</v>
+        <v>4.840411989265054e-5</v>
       </c>
       <c r="E2">
-        <v>-4.0248493744597103E-8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-4.02484937445971e-8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
-        <v>-1.0798671662802532E-44</v>
+        <v>-1.0798671662802532e-44</v>
       </c>
       <c r="C3">
-        <v>-5.3681075337507593E-36</v>
+        <v>-5.368107533750759e-36</v>
       </c>
       <c r="D3">
-        <v>3.1539921415434568E-33</v>
+        <v>3.153992141543457e-33</v>
       </c>
       <c r="E3">
-        <v>-2.7795515648053547E-36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-2.7795515648053547e-36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
-        <v>1.3577067628692752E-43</v>
+        <v>1.3577067628692752e-43</v>
       </c>
       <c r="C4">
-        <v>1.4648995799039157E-34</v>
+        <v>1.4648995799039157e-34</v>
       </c>
       <c r="D4">
-        <v>-6.4414320850285898E-26</v>
+        <v>-6.44143208502859e-26</v>
       </c>
       <c r="E4">
-        <v>7.6036980235573947E-35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.603698023557395e-35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5">
-        <v>-3.8892624661201705E-42</v>
+        <v>-3.8892624661201705e-42</v>
       </c>
       <c r="C5">
-        <v>-7.0570465655800507E-38</v>
+        <v>-7.057046565580051e-38</v>
       </c>
       <c r="D5">
-        <v>-2.1154740576433757E-25</v>
+        <v>-2.1154740576433757e-25</v>
       </c>
       <c r="E5">
-        <v>9.1408163871718978E-38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9.140816387171898e-38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1047,50 +1042,50 @@
         <v>1.9483599994726992</v>
       </c>
       <c r="C6">
-        <v>8.0447231349822682E-7</v>
+        <v>8.044723134982268e-7</v>
       </c>
       <c r="D6">
-        <v>8.2892802669848882E-7</v>
+        <v>8.289280266984888e-7</v>
       </c>
       <c r="E6">
-        <v>-6.858815218150862E-10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-6.858815218150862e-10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7">
-        <v>8.8693999975996007</v>
+        <v>8.8693999975996</v>
       </c>
       <c r="C7">
-        <v>3.6621496507690296E-6</v>
+        <v>3.6621496507690296e-6</v>
       </c>
       <c r="D7">
-        <v>3.7735635515709186E-6</v>
+        <v>3.7735635515709186e-6</v>
       </c>
       <c r="E7">
-        <v>-3.1442782525547759E-9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.144278252554776e-9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8">
-        <v>9.7417999973634952</v>
+        <v>9.741799997363495</v>
       </c>
       <c r="C8">
-        <v>4.0223618729174193E-6</v>
+        <v>4.022361872917419e-6</v>
       </c>
       <c r="D8">
-        <v>4.1452745471998227E-6</v>
+        <v>4.145274547199823e-6</v>
       </c>
       <c r="E8">
-        <v>-3.3630662278504839E-9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.363066227850484e-9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1098,16 +1093,16 @@
         <v>3.6059199990240995</v>
       </c>
       <c r="C9">
-        <v>1.4888744971323444E-6</v>
+        <v>1.4888744971323444e-6</v>
       </c>
       <c r="D9">
-        <v>1.5344810644875359E-6</v>
+        <v>1.5344810644875359e-6</v>
       </c>
       <c r="E9">
-        <v>-1.2634516469754283E-9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.2634516469754283e-9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1115,33 +1110,33 @@
         <v>2.0501399994451535</v>
       </c>
       <c r="C10">
-        <v>8.4649701166386379E-7</v>
+        <v>8.464970116638638e-7</v>
       </c>
       <c r="D10">
-        <v>8.7199825036180915E-7</v>
+        <v>8.719982503618091e-7</v>
       </c>
       <c r="E10">
-        <v>-7.1052223414578668E-10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-7.105222341457867e-10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11">
-        <v>5.3361799985558251</v>
+        <v>5.336179998555825</v>
       </c>
       <c r="C11">
-        <v>2.2032943659455907E-6</v>
+        <v>2.2032943659455907e-6</v>
       </c>
       <c r="D11">
-        <v>2.270798547788992E-6</v>
+        <v>2.270798547788992e-6</v>
       </c>
       <c r="E11">
-        <v>-1.8548313448602313E-9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.8548313448602313e-9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1149,67 +1144,67 @@
         <v>113.76095996921192</v>
       </c>
       <c r="C12">
-        <v>4.6971578963950364E-5</v>
+        <v>4.6971578963950364e-5</v>
       </c>
       <c r="D12">
-        <v>4.8404119892650542E-5</v>
+        <v>4.840411989265054e-5</v>
       </c>
       <c r="E12">
-        <v>-4.0248493744597103E-8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-4.02484937445971e-8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13">
-        <v>716.82199382956378</v>
+        <v>716.8219938295638</v>
       </c>
       <c r="C13">
-        <v>3.4684914754603167E-3</v>
+        <v>0.0034684914754603167</v>
       </c>
       <c r="D13">
         <v>0.34907069314935024</v>
       </c>
       <c r="E13">
-        <v>-3.4258103152575114E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.00034258103152575114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14">
-        <v>2.0549998498816777E-43</v>
+        <v>2.0549998498816777e-43</v>
       </c>
       <c r="C14">
-        <v>-7.3229666110423908E-35</v>
+        <v>-7.322966611042391e-35</v>
       </c>
       <c r="D14">
-        <v>-3.2207074370080907E-26</v>
+        <v>-3.2207074370080907e-26</v>
       </c>
       <c r="E14">
-        <v>-3.7874616981304386E-35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.7874616981304386e-35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15">
-        <v>2.083252539316061E-42</v>
+        <v>2.083252539316061e-42</v>
       </c>
       <c r="C15">
-        <v>-1.2901630370691447E-34</v>
+        <v>-1.2901630370691447e-34</v>
       </c>
       <c r="D15">
-        <v>-9.6779589337653902E-26</v>
+        <v>-9.67795893376539e-26</v>
       </c>
       <c r="E15">
-        <v>-6.6798478715653673E-35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-6.679847871565367e-35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1217,50 +1212,50 @@
         <v>1.9483599994726992</v>
       </c>
       <c r="C16">
-        <v>8.0447231349822682E-7</v>
+        <v>8.044723134982268e-7</v>
       </c>
       <c r="D16">
-        <v>8.2892802669848882E-7</v>
+        <v>8.289280266984888e-7</v>
       </c>
       <c r="E16">
-        <v>-6.858815218150862E-10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-6.858815218150862e-10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17">
-        <v>8.8693999975996007</v>
+        <v>8.8693999975996</v>
       </c>
       <c r="C17">
-        <v>3.6621496507690296E-6</v>
+        <v>3.6621496507690296e-6</v>
       </c>
       <c r="D17">
-        <v>3.7735635515709186E-6</v>
+        <v>3.7735635515709186e-6</v>
       </c>
       <c r="E17">
-        <v>-3.1442782525547759E-9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.144278252554776e-9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="B18">
-        <v>9.7417999973634952</v>
+        <v>9.741799997363495</v>
       </c>
       <c r="C18">
-        <v>4.0223618729174193E-6</v>
+        <v>4.022361872917419e-6</v>
       </c>
       <c r="D18">
-        <v>4.1452745471998227E-6</v>
+        <v>4.145274547199823e-6</v>
       </c>
       <c r="E18">
-        <v>-3.3630662278504839E-9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.363066227850484e-9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1268,16 +1263,16 @@
         <v>3.6059199990240995</v>
       </c>
       <c r="C19">
-        <v>1.4888744971323444E-6</v>
+        <v>1.4888744971323444e-6</v>
       </c>
       <c r="D19">
-        <v>1.5344810644875359E-6</v>
+        <v>1.5344810644875359e-6</v>
       </c>
       <c r="E19">
-        <v>-1.2634516469754283E-9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.2634516469754283e-9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1285,33 +1280,33 @@
         <v>2.0501399994451535</v>
       </c>
       <c r="C20">
-        <v>8.4649701166386379E-7</v>
+        <v>8.464970116638638e-7</v>
       </c>
       <c r="D20">
-        <v>8.7199825036180915E-7</v>
+        <v>8.719982503618091e-7</v>
       </c>
       <c r="E20">
-        <v>-7.1052223414578668E-10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-7.105222341457867e-10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>24</v>
       </c>
       <c r="B21">
-        <v>5.3361799985558251</v>
+        <v>5.336179998555825</v>
       </c>
       <c r="C21">
-        <v>2.2032943659455907E-6</v>
+        <v>2.2032943659455907e-6</v>
       </c>
       <c r="D21">
-        <v>2.270798547788992E-6</v>
+        <v>2.270798547788992e-6</v>
       </c>
       <c r="E21">
-        <v>-1.8548313448602313E-9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.8548313448602313e-9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1319,67 +1314,67 @@
         <v>113.76095996921192</v>
       </c>
       <c r="C22">
-        <v>4.6971578963950364E-5</v>
+        <v>4.6971578963950364e-5</v>
       </c>
       <c r="D22">
-        <v>4.8404119892650542E-5</v>
+        <v>4.840411989265054e-5</v>
       </c>
       <c r="E22">
-        <v>-4.0248493744597103E-8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-4.02484937445971e-8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>26</v>
       </c>
       <c r="B23">
-        <v>716.82199382956378</v>
+        <v>716.8219938295638</v>
       </c>
       <c r="C23">
-        <v>3.4684914754603167E-3</v>
+        <v>0.0034684914754603167</v>
       </c>
       <c r="D23">
         <v>0.34907069314935024</v>
       </c>
       <c r="E23">
-        <v>-3.4258103152575114E-4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.00034258103152575114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>27</v>
       </c>
       <c r="B24">
-        <v>2.1014708141234524E-42</v>
+        <v>2.1014708141234524e-42</v>
       </c>
       <c r="C24">
-        <v>-3.4293919571991376E-38</v>
+        <v>-3.4293919571991376e-38</v>
       </c>
       <c r="D24">
-        <v>-5.3047016862421695E-26</v>
+        <v>-5.30470168624217e-26</v>
       </c>
       <c r="E24">
-        <v>-3.0090309171974163E-37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.0090309171974163e-37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>28</v>
       </c>
       <c r="B25">
-        <v>3.6424306022568E-42</v>
+        <v>3.6424306022568e-42</v>
       </c>
       <c r="C25">
-        <v>-2.5796628257899508E-34</v>
+        <v>-2.579662825789951e-34</v>
       </c>
       <c r="D25">
-        <v>2.6697990291276402E-26</v>
+        <v>2.66979902912764e-26</v>
       </c>
       <c r="E25">
-        <v>-1.3354098108927875E-34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.3354098108927875e-34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1387,50 +1382,50 @@
         <v>1.9483599994726992</v>
       </c>
       <c r="C26">
-        <v>8.0447231349822682E-7</v>
+        <v>8.044723134982268e-7</v>
       </c>
       <c r="D26">
-        <v>8.2892802669848882E-7</v>
+        <v>8.289280266984888e-7</v>
       </c>
       <c r="E26">
-        <v>-6.858815218150862E-10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-6.858815218150862e-10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>30</v>
       </c>
       <c r="B27">
-        <v>8.8693999975996007</v>
+        <v>8.8693999975996</v>
       </c>
       <c r="C27">
-        <v>3.6621496507690296E-6</v>
+        <v>3.6621496507690296e-6</v>
       </c>
       <c r="D27">
-        <v>3.7735635515709186E-6</v>
+        <v>3.7735635515709186e-6</v>
       </c>
       <c r="E27">
-        <v>-3.1442782525547759E-9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.144278252554776e-9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>31</v>
       </c>
       <c r="B28">
-        <v>9.7417999973634952</v>
+        <v>9.741799997363495</v>
       </c>
       <c r="C28">
-        <v>4.0223618729174193E-6</v>
+        <v>4.022361872917419e-6</v>
       </c>
       <c r="D28">
-        <v>4.1452745471998227E-6</v>
+        <v>4.145274547199823e-6</v>
       </c>
       <c r="E28">
-        <v>-3.3630662278504839E-9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.363066227850484e-9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1438,16 +1433,16 @@
         <v>3.6059199990240995</v>
       </c>
       <c r="C29">
-        <v>1.4888744971323444E-6</v>
+        <v>1.4888744971323444e-6</v>
       </c>
       <c r="D29">
-        <v>1.5344810644875359E-6</v>
+        <v>1.5344810644875359e-6</v>
       </c>
       <c r="E29">
-        <v>-1.2634516469754283E-9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.2634516469754283e-9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1455,33 +1450,33 @@
         <v>2.0501399994451535</v>
       </c>
       <c r="C30">
-        <v>8.4649701166386379E-7</v>
+        <v>8.464970116638638e-7</v>
       </c>
       <c r="D30">
-        <v>8.7199825036180915E-7</v>
+        <v>8.719982503618091e-7</v>
       </c>
       <c r="E30">
-        <v>-7.1052223414578668E-10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-7.105222341457867e-10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>34</v>
       </c>
       <c r="B31">
-        <v>5.3361799985558251</v>
+        <v>5.336179998555825</v>
       </c>
       <c r="C31">
-        <v>2.2032943659455907E-6</v>
+        <v>2.2032943659455907e-6</v>
       </c>
       <c r="D31">
-        <v>2.270798547788992E-6</v>
+        <v>2.270798547788992e-6</v>
       </c>
       <c r="E31">
-        <v>-1.8548313448602313E-9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.8548313448602313e-9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1489,67 +1484,67 @@
         <v>113.76095996921192</v>
       </c>
       <c r="C32">
-        <v>4.6971578963950364E-5</v>
+        <v>4.6971578963950364e-5</v>
       </c>
       <c r="D32">
-        <v>4.8404119892650542E-5</v>
+        <v>4.840411989265054e-5</v>
       </c>
       <c r="E32">
-        <v>-4.0248493744597103E-8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-4.02484937445971e-8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>36</v>
       </c>
       <c r="B33">
-        <v>716.82199382956378</v>
+        <v>716.8219938295638</v>
       </c>
       <c r="C33">
-        <v>3.4684914754603167E-3</v>
+        <v>0.0034684914754603167</v>
       </c>
       <c r="D33">
         <v>0.34907069314935024</v>
       </c>
       <c r="E33">
-        <v>-3.4258103152575114E-4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.00034258103152575114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>37</v>
       </c>
       <c r="B34">
-        <v>1.7695986017706285E-42</v>
+        <v>1.7695986017706285e-42</v>
       </c>
       <c r="C34">
-        <v>3.6609630528707902E-35</v>
+        <v>3.66096305287079e-35</v>
       </c>
       <c r="D34">
-        <v>9.4724665121415325E-28</v>
+        <v>9.472466512141533e-28</v>
       </c>
       <c r="E34">
-        <v>1.881620541681442E-35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.881620541681442e-35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>38</v>
       </c>
       <c r="B35">
-        <v>-1.2378175786874966E-42</v>
+        <v>-1.2378175786874966e-42</v>
       </c>
       <c r="C35">
-        <v>-2.6903027677569266E-34</v>
+        <v>-2.6903027677569266e-34</v>
       </c>
       <c r="D35">
-        <v>-2.2272026306163275E-25</v>
+        <v>-2.2272026306163275e-25</v>
       </c>
       <c r="E35">
-        <v>-1.390862291978149E-34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.390862291978149e-34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1557,50 +1552,50 @@
         <v>1.9483599994726992</v>
       </c>
       <c r="C36">
-        <v>8.0447231349822682E-7</v>
+        <v>8.044723134982268e-7</v>
       </c>
       <c r="D36">
-        <v>8.2892802669848882E-7</v>
+        <v>8.289280266984888e-7</v>
       </c>
       <c r="E36">
-        <v>-6.858815218150862E-10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-6.858815218150862e-10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>40</v>
       </c>
       <c r="B37">
-        <v>8.8693999975996007</v>
+        <v>8.8693999975996</v>
       </c>
       <c r="C37">
-        <v>3.6621496507690296E-6</v>
+        <v>3.6621496507690296e-6</v>
       </c>
       <c r="D37">
-        <v>3.7735635515709186E-6</v>
+        <v>3.7735635515709186e-6</v>
       </c>
       <c r="E37">
-        <v>-3.1442782525547759E-9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.144278252554776e-9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>41</v>
       </c>
       <c r="B38">
-        <v>9.7417999973634952</v>
+        <v>9.741799997363495</v>
       </c>
       <c r="C38">
-        <v>4.0223618729174193E-6</v>
+        <v>4.022361872917419e-6</v>
       </c>
       <c r="D38">
-        <v>4.1452745471998227E-6</v>
+        <v>4.145274547199823e-6</v>
       </c>
       <c r="E38">
-        <v>-3.3630662278504839E-9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.363066227850484e-9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1608,16 +1603,16 @@
         <v>3.6059199990240995</v>
       </c>
       <c r="C39">
-        <v>1.4888744971323444E-6</v>
+        <v>1.4888744971323444e-6</v>
       </c>
       <c r="D39">
-        <v>1.5344810644875359E-6</v>
+        <v>1.5344810644875359e-6</v>
       </c>
       <c r="E39">
-        <v>-1.2634516469754283E-9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.2634516469754283e-9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -1625,33 +1620,33 @@
         <v>2.0501399994451535</v>
       </c>
       <c r="C40">
-        <v>8.4649701166386379E-7</v>
+        <v>8.464970116638638e-7</v>
       </c>
       <c r="D40">
-        <v>8.7199825036180915E-7</v>
+        <v>8.719982503618091e-7</v>
       </c>
       <c r="E40">
-        <v>-7.1052223414578668E-10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-7.105222341457867e-10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>44</v>
       </c>
       <c r="B41">
-        <v>5.3361799985558251</v>
+        <v>5.336179998555825</v>
       </c>
       <c r="C41">
-        <v>2.2032943659455907E-6</v>
+        <v>2.2032943659455907e-6</v>
       </c>
       <c r="D41">
-        <v>2.270798547788992E-6</v>
+        <v>2.270798547788992e-6</v>
       </c>
       <c r="E41">
-        <v>-1.8548313448602313E-9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.8548313448602313e-9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -1659,67 +1654,67 @@
         <v>113.76095996921192</v>
       </c>
       <c r="C42">
-        <v>4.6971578963950364E-5</v>
+        <v>4.6971578963950364e-5</v>
       </c>
       <c r="D42">
-        <v>4.8404119892650542E-5</v>
+        <v>4.840411989265054e-5</v>
       </c>
       <c r="E42">
-        <v>-4.0248493744597103E-8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-4.02484937445971e-8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>46</v>
       </c>
       <c r="B43">
-        <v>716.82199382956378</v>
+        <v>716.8219938295638</v>
       </c>
       <c r="C43">
-        <v>3.4684914754603167E-3</v>
+        <v>0.0034684914754603167</v>
       </c>
       <c r="D43">
         <v>0.34907069314935024</v>
       </c>
       <c r="E43">
-        <v>-3.4258103152575114E-4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.00034258103152575114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>47</v>
       </c>
       <c r="B44">
-        <v>9.7631897850653208E-43</v>
+        <v>9.763189785065321e-43</v>
       </c>
       <c r="C44">
-        <v>-1.4648248359084601E-34</v>
+        <v>-1.46482483590846e-34</v>
       </c>
       <c r="D44">
-        <v>6.0625248191187222E-26</v>
+        <v>6.062524819118722e-26</v>
       </c>
       <c r="E44">
-        <v>-7.5754329438324499E-35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-7.57543294383245e-35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>48</v>
       </c>
       <c r="B45">
-        <v>7.89677127326731E-43</v>
+        <v>7.89677127326731e-43</v>
       </c>
       <c r="C45">
-        <v>-8.0708146173046137E-34</v>
+        <v>-8.070814617304614e-34</v>
       </c>
       <c r="D45">
-        <v>-8.3519683700428957E-26</v>
+        <v>-8.351968370042896e-26</v>
       </c>
       <c r="E45">
-        <v>-4.1739557797937996E-34</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-4.1739557797938e-34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -1727,50 +1722,50 @@
         <v>1.9483599994726992</v>
       </c>
       <c r="C46">
-        <v>8.0447231349822682E-7</v>
+        <v>8.044723134982268e-7</v>
       </c>
       <c r="D46">
-        <v>8.2892802669848882E-7</v>
+        <v>8.289280266984888e-7</v>
       </c>
       <c r="E46">
-        <v>-6.858815218150862E-10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-6.858815218150862e-10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>50</v>
       </c>
       <c r="B47">
-        <v>8.8693999975996007</v>
+        <v>8.8693999975996</v>
       </c>
       <c r="C47">
-        <v>3.6621496507690296E-6</v>
+        <v>3.6621496507690296e-6</v>
       </c>
       <c r="D47">
-        <v>3.7735635515709186E-6</v>
+        <v>3.7735635515709186e-6</v>
       </c>
       <c r="E47">
-        <v>-3.1442782525547759E-9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.144278252554776e-9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>51</v>
       </c>
       <c r="B48">
-        <v>9.7417999973634952</v>
+        <v>9.741799997363495</v>
       </c>
       <c r="C48">
-        <v>4.0223618729174193E-6</v>
+        <v>4.022361872917419e-6</v>
       </c>
       <c r="D48">
-        <v>4.1452745471998227E-6</v>
+        <v>4.145274547199823e-6</v>
       </c>
       <c r="E48">
-        <v>-3.3630662278504839E-9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.363066227850484e-9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1778,16 +1773,16 @@
         <v>3.6059199990240995</v>
       </c>
       <c r="C49">
-        <v>1.4888744971323444E-6</v>
+        <v>1.4888744971323444e-6</v>
       </c>
       <c r="D49">
-        <v>1.5344810644875359E-6</v>
+        <v>1.5344810644875359e-6</v>
       </c>
       <c r="E49">
-        <v>-1.2634516469754283E-9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.2634516469754283e-9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -1795,33 +1790,33 @@
         <v>2.0501399994451535</v>
       </c>
       <c r="C50">
-        <v>8.4649701166386379E-7</v>
+        <v>8.464970116638638e-7</v>
       </c>
       <c r="D50">
-        <v>8.7199825036180915E-7</v>
+        <v>8.719982503618091e-7</v>
       </c>
       <c r="E50">
-        <v>-7.1052223414578668E-10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-7.105222341457867e-10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>54</v>
       </c>
       <c r="B51">
-        <v>5.3361799985558251</v>
+        <v>5.336179998555825</v>
       </c>
       <c r="C51">
-        <v>2.2032943659455907E-6</v>
+        <v>2.2032943659455907e-6</v>
       </c>
       <c r="D51">
-        <v>2.270798547788992E-6</v>
+        <v>2.270798547788992e-6</v>
       </c>
       <c r="E51">
-        <v>-1.8548313448602313E-9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.8548313448602313e-9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -1829,33 +1824,33 @@
         <v>179.52172526328644</v>
       </c>
       <c r="C52">
-        <v>3.259598334038693E-5</v>
+        <v>3.259598334038693e-5</v>
       </c>
       <c r="D52">
-        <v>-4.4547079146595239E-3</v>
+        <v>-0.004454707914659524</v>
       </c>
       <c r="E52">
-        <v>4.399172902243834E-6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4.399172902243834e-6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>56</v>
       </c>
       <c r="B53">
-        <v>656.03269609703091</v>
+        <v>656.0326960970309</v>
       </c>
       <c r="C53">
-        <v>3.3601090013836445E-3</v>
+        <v>0.0033601090013836445</v>
       </c>
       <c r="D53">
-        <v>0.33995645225097021</v>
+        <v>0.3399564522509702</v>
       </c>
       <c r="E53">
-        <v>-3.3360789330587841E-4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.0003336078933058784</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -1863,16 +1858,16 @@
         <v>55.140547110317776</v>
       </c>
       <c r="C54">
-        <v>1.8910623529187361E-4</v>
+        <v>0.0001891062352918736</v>
       </c>
       <c r="D54">
-        <v>1.8174136552332392E-2</v>
+        <v>0.018174136552332392</v>
       </c>
       <c r="E54">
-        <v>-1.7893768581144359E-5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.789376858114436e-5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -1880,118 +1875,118 @@
         <v>0.22785162720980615</v>
       </c>
       <c r="C55">
-        <v>-1.326471962948949E-7</v>
+        <v>-1.326471962948949e-7</v>
       </c>
       <c r="D55">
-        <v>-2.6176277646587095E-5</v>
+        <v>-2.6176277646587095e-5</v>
       </c>
       <c r="E55">
-        <v>2.5124156933715828E-8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.5124156933715828e-8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>59</v>
       </c>
       <c r="B56">
-        <v>32.229083052134222</v>
+        <v>32.22908305213422</v>
       </c>
       <c r="C56">
-        <v>5.5062044327101691E-5</v>
+        <v>5.506204432710169e-5</v>
       </c>
       <c r="D56">
-        <v>4.5710729638432108E-3</v>
+        <v>0.004571072963843211</v>
       </c>
       <c r="E56">
-        <v>-4.4994351923157284E-6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-4.499435192315728e-6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>60</v>
       </c>
       <c r="B57">
-        <v>7.0730723599945638E-17</v>
+        <v>7.073072359994564e-17</v>
       </c>
       <c r="C57">
-        <v>-1.5806407997613857E-13</v>
+        <v>-1.5806407997613857e-13</v>
       </c>
       <c r="D57">
-        <v>2.7056654528446611E-11</v>
+        <v>2.705665452844661e-11</v>
       </c>
       <c r="E57">
-        <v>2.0158769258725188E-11</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.015876925872519e-11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>61</v>
       </c>
       <c r="B58">
-        <v>7.0730723599945613E-17</v>
+        <v>7.073072359994561e-17</v>
       </c>
       <c r="C58">
-        <v>-2.202204832463742E-13</v>
+        <v>-2.202204832463742e-13</v>
       </c>
       <c r="D58">
-        <v>-4.9068400131251812E-10</v>
+        <v>-4.906840013125181e-10</v>
       </c>
       <c r="E58">
-        <v>1.8802088481273723E-11</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.8802088481273723e-11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>62</v>
       </c>
       <c r="B59">
-        <v>4.3484744181208512E-17</v>
+        <v>4.348474418120851e-17</v>
       </c>
       <c r="C59">
-        <v>-1.2066720500484019E-13</v>
+        <v>-1.206672050048402e-13</v>
       </c>
       <c r="D59">
-        <v>8.7595775051973687E-12</v>
+        <v>8.759577505197369e-12</v>
       </c>
       <c r="E59">
-        <v>3.9561939820912782E-12</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.956193982091278e-12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>63</v>
       </c>
       <c r="B60">
-        <v>4.3484744181208512E-17</v>
+        <v>4.348474418120851e-17</v>
       </c>
       <c r="C60">
-        <v>-7.324733433515021E-14</v>
+        <v>-7.324733433515021e-14</v>
       </c>
       <c r="D60">
-        <v>-3.3002372003102834E-11</v>
+        <v>-3.3002372003102834e-11</v>
       </c>
       <c r="E60">
-        <v>-4.2201644083458693E-12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-4.220164408345869e-12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>64</v>
       </c>
       <c r="B61">
-        <v>-4.3848028505915892E-16</v>
+        <v>-4.384802850591589e-16</v>
       </c>
       <c r="C61">
-        <v>3.4653697035623437E-13</v>
+        <v>3.4653697035623437e-13</v>
       </c>
       <c r="D61">
-        <v>1.910694672295929E-10</v>
+        <v>1.910694672295929e-10</v>
       </c>
       <c r="E61">
-        <v>3.0586160148583495E-12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.0586160148583495e-12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -1999,33 +1994,33 @@
         <v>179.52172526328644</v>
       </c>
       <c r="C62">
-        <v>3.259598334038693E-5</v>
+        <v>3.259598334038693e-5</v>
       </c>
       <c r="D62">
-        <v>-4.4547079146595239E-3</v>
+        <v>-0.004454707914659524</v>
       </c>
       <c r="E62">
-        <v>4.399172902243834E-6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4.399172902243834e-6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>66</v>
       </c>
       <c r="B63">
-        <v>656.03269609703091</v>
+        <v>656.0326960970309</v>
       </c>
       <c r="C63">
-        <v>3.3601090013836445E-3</v>
+        <v>0.0033601090013836445</v>
       </c>
       <c r="D63">
-        <v>0.33995645225097021</v>
+        <v>0.3399564522509702</v>
       </c>
       <c r="E63">
-        <v>-3.3360789330587841E-4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.0003336078933058784</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -2033,16 +2028,16 @@
         <v>55.140547110317776</v>
       </c>
       <c r="C64">
-        <v>1.8910623529187361E-4</v>
+        <v>0.0001891062352918736</v>
       </c>
       <c r="D64">
-        <v>1.8174136552332392E-2</v>
+        <v>0.018174136552332392</v>
       </c>
       <c r="E64">
-        <v>-1.7893768581144359E-5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.789376858114436e-5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -2050,33 +2045,33 @@
         <v>0.22785162720980615</v>
       </c>
       <c r="C65">
-        <v>-1.326471962948949E-7</v>
+        <v>-1.326471962948949e-7</v>
       </c>
       <c r="D65">
-        <v>-2.6176277646587095E-5</v>
+        <v>-2.6176277646587095e-5</v>
       </c>
       <c r="E65">
-        <v>2.5124156933715828E-8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.5124156933715828e-8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>69</v>
       </c>
       <c r="B66">
-        <v>32.229083052134222</v>
+        <v>32.22908305213422</v>
       </c>
       <c r="C66">
-        <v>5.5062044327101691E-5</v>
+        <v>5.506204432710169e-5</v>
       </c>
       <c r="D66">
-        <v>4.5710729638432108E-3</v>
+        <v>0.004571072963843211</v>
       </c>
       <c r="E66">
-        <v>-4.4994351923157284E-6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-4.499435192315728e-6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -2084,33 +2079,33 @@
         <v>179.52172526328644</v>
       </c>
       <c r="C67">
-        <v>3.259598334038693E-5</v>
+        <v>3.259598334038693e-5</v>
       </c>
       <c r="D67">
-        <v>-4.4547079146595239E-3</v>
+        <v>-0.004454707914659524</v>
       </c>
       <c r="E67">
-        <v>4.399172902243834E-6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4.399172902243834e-6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>71</v>
       </c>
       <c r="B68">
-        <v>656.03269609703091</v>
+        <v>656.0326960970309</v>
       </c>
       <c r="C68">
-        <v>3.3601090013836445E-3</v>
+        <v>0.0033601090013836445</v>
       </c>
       <c r="D68">
-        <v>0.33995645225097021</v>
+        <v>0.3399564522509702</v>
       </c>
       <c r="E68">
-        <v>-3.3360789330587841E-4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.0003336078933058784</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>72</v>
       </c>
@@ -2118,16 +2113,16 @@
         <v>55.140547110317776</v>
       </c>
       <c r="C69">
-        <v>1.8910623529187361E-4</v>
+        <v>0.0001891062352918736</v>
       </c>
       <c r="D69">
-        <v>1.8174136552332392E-2</v>
+        <v>0.018174136552332392</v>
       </c>
       <c r="E69">
-        <v>-1.7893768581144359E-5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.789376858114436e-5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>73</v>
       </c>
@@ -2135,33 +2130,33 @@
         <v>0.22785162720980615</v>
       </c>
       <c r="C70">
-        <v>-1.326471962948949E-7</v>
+        <v>-1.326471962948949e-7</v>
       </c>
       <c r="D70">
-        <v>-2.6176277646587095E-5</v>
+        <v>-2.6176277646587095e-5</v>
       </c>
       <c r="E70">
-        <v>2.5124156933715828E-8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.5124156933715828e-8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>74</v>
       </c>
       <c r="B71">
-        <v>32.229083052134222</v>
+        <v>32.22908305213422</v>
       </c>
       <c r="C71">
-        <v>5.5062044327101691E-5</v>
+        <v>5.506204432710169e-5</v>
       </c>
       <c r="D71">
-        <v>4.5710729638432108E-3</v>
+        <v>0.004571072963843211</v>
       </c>
       <c r="E71">
-        <v>-4.4994351923157284E-6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-4.499435192315728e-6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>75</v>
       </c>
@@ -2169,33 +2164,33 @@
         <v>179.52172526328644</v>
       </c>
       <c r="C72">
-        <v>3.259598334038693E-5</v>
+        <v>3.259598334038693e-5</v>
       </c>
       <c r="D72">
-        <v>-4.4547079146595239E-3</v>
+        <v>-0.004454707914659524</v>
       </c>
       <c r="E72">
-        <v>4.399172902243834E-6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4.399172902243834e-6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>76</v>
       </c>
       <c r="B73">
-        <v>656.03269609703091</v>
+        <v>656.0326960970309</v>
       </c>
       <c r="C73">
-        <v>3.3601090013836445E-3</v>
+        <v>0.0033601090013836445</v>
       </c>
       <c r="D73">
-        <v>0.33995645225097021</v>
+        <v>0.3399564522509702</v>
       </c>
       <c r="E73">
-        <v>-3.3360789330587841E-4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.0003336078933058784</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>77</v>
       </c>
@@ -2203,16 +2198,16 @@
         <v>55.140547110317776</v>
       </c>
       <c r="C74">
-        <v>1.8910623529187361E-4</v>
+        <v>0.0001891062352918736</v>
       </c>
       <c r="D74">
-        <v>1.8174136552332392E-2</v>
+        <v>0.018174136552332392</v>
       </c>
       <c r="E74">
-        <v>-1.7893768581144359E-5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.789376858114436e-5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>78</v>
       </c>
@@ -2220,67 +2215,67 @@
         <v>0.22785162720980615</v>
       </c>
       <c r="C75">
-        <v>-1.326471962948949E-7</v>
+        <v>-1.326471962948949e-7</v>
       </c>
       <c r="D75">
-        <v>-2.6176277646587095E-5</v>
+        <v>-2.6176277646587095e-5</v>
       </c>
       <c r="E75">
-        <v>2.5124156933715828E-8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.5124156933715828e-8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>79</v>
       </c>
       <c r="B76">
-        <v>32.229083052134222</v>
+        <v>32.22908305213422</v>
       </c>
       <c r="C76">
-        <v>5.5062044327101691E-5</v>
+        <v>5.506204432710169e-5</v>
       </c>
       <c r="D76">
-        <v>4.5710729638432108E-3</v>
+        <v>0.004571072963843211</v>
       </c>
       <c r="E76">
-        <v>-4.4994351923157284E-6</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-4.499435192315728e-6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>80</v>
       </c>
       <c r="B77">
-        <v>94.625821146436223</v>
+        <v>94.62582114643622</v>
       </c>
       <c r="C77">
-        <v>-2.3729494949245651E-4</v>
+        <v>-0.0002372949494924565</v>
       </c>
       <c r="D77">
-        <v>-2.8720270960206594E-2</v>
+        <v>-0.028720270960206594</v>
       </c>
       <c r="E77">
-        <v>2.8250883617757481E-5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.825088361775748e-5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>81</v>
       </c>
       <c r="B78">
-        <v>518.61805996236171</v>
+        <v>518.6180599623617</v>
       </c>
       <c r="C78">
-        <v>2.8634557240236665E-3</v>
+        <v>0.0028634557240236665</v>
       </c>
       <c r="D78">
-        <v>0.29345798611010632</v>
+        <v>0.2934579861101063</v>
       </c>
       <c r="E78">
-        <v>-2.8793730469314018E-4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.0002879373046931402</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>82</v>
       </c>
@@ -2288,84 +2283,84 @@
         <v>362.34699147868747</v>
       </c>
       <c r="C79">
-        <v>1.2255412854679871E-3</v>
+        <v>0.001225541285467987</v>
       </c>
       <c r="D79">
         <v>0.11320366788086986</v>
       </c>
       <c r="E79">
-        <v>-1.1126692945545275E-4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.00011126692945545275</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>83</v>
       </c>
       <c r="B80">
-        <v>32.605023726241001</v>
+        <v>32.605023726241</v>
       </c>
       <c r="C80">
-        <v>4.2996060683729675E-5</v>
+        <v>4.2996060683729675e-5</v>
       </c>
       <c r="D80">
-        <v>2.0065054011491469E-3</v>
+        <v>0.002006505401149147</v>
       </c>
       <c r="E80">
-        <v>-2.0096134882036183E-6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-2.0096134882036183e-6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>84</v>
       </c>
       <c r="B81">
-        <v>84.747815069953248</v>
+        <v>84.74781506995325</v>
       </c>
       <c r="C81">
-        <v>2.8182426668380266E-4</v>
+        <v>0.00028182426668380266</v>
       </c>
       <c r="D81">
-        <v>2.680393545685095E-2</v>
+        <v>0.02680393545685095</v>
       </c>
       <c r="E81">
-        <v>-2.6316614750290048E-5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-2.6316614750290048e-5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>85</v>
       </c>
       <c r="B82">
-        <v>94.625821146436223</v>
+        <v>94.62582114643622</v>
       </c>
       <c r="C82">
-        <v>-2.3729494949245651E-4</v>
+        <v>-0.0002372949494924565</v>
       </c>
       <c r="D82">
-        <v>-2.8720270960206594E-2</v>
+        <v>-0.028720270960206594</v>
       </c>
       <c r="E82">
-        <v>2.8250883617757481E-5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.825088361775748e-5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>86</v>
       </c>
       <c r="B83">
-        <v>518.61805996236171</v>
+        <v>518.6180599623617</v>
       </c>
       <c r="C83">
-        <v>2.8634557240236665E-3</v>
+        <v>0.0028634557240236665</v>
       </c>
       <c r="D83">
-        <v>0.29345798611010632</v>
+        <v>0.2934579861101063</v>
       </c>
       <c r="E83">
-        <v>-2.8793730469314018E-4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.0002879373046931402</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>87</v>
       </c>
@@ -2373,50 +2368,50 @@
         <v>362.34699147868747</v>
       </c>
       <c r="C84">
-        <v>1.2255412854679871E-3</v>
+        <v>0.001225541285467987</v>
       </c>
       <c r="D84">
         <v>0.11320366788086986</v>
       </c>
       <c r="E84">
-        <v>-1.1126692945545275E-4</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.00011126692945545275</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>88</v>
       </c>
       <c r="B85">
-        <v>32.605023726241001</v>
+        <v>32.605023726241</v>
       </c>
       <c r="C85">
-        <v>4.2996060683729675E-5</v>
+        <v>4.2996060683729675e-5</v>
       </c>
       <c r="D85">
-        <v>2.0065054011491469E-3</v>
+        <v>0.002006505401149147</v>
       </c>
       <c r="E85">
-        <v>-2.0096134882036183E-6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-2.0096134882036183e-6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>89</v>
       </c>
       <c r="B86">
-        <v>84.747815069953248</v>
+        <v>84.74781506995325</v>
       </c>
       <c r="C86">
-        <v>2.8182426668380266E-4</v>
+        <v>0.00028182426668380266</v>
       </c>
       <c r="D86">
-        <v>2.680393545685095E-2</v>
+        <v>0.02680393545685095</v>
       </c>
       <c r="E86">
-        <v>-2.6316614750290048E-5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-2.6316614750290048e-5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>90</v>
       </c>
@@ -2424,50 +2419,50 @@
         <v>0.30066254435730366</v>
       </c>
       <c r="C87">
-        <v>-2.851398607942417E-6</v>
+        <v>-2.851398607942417e-6</v>
       </c>
       <c r="D87">
-        <v>-3.1017548591837898E-4</v>
+        <v>-0.000310175485918379</v>
       </c>
       <c r="E87">
-        <v>3.0613332341107063E-7</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.0613332341107063e-7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>91</v>
       </c>
       <c r="B88">
-        <v>582.93357348816028</v>
+        <v>582.9335734881603</v>
       </c>
       <c r="C88">
-        <v>3.1237528626846486E-3</v>
+        <v>0.0031237528626846486</v>
       </c>
       <c r="D88">
-        <v>0.31783666233027408</v>
+        <v>0.3178366623302741</v>
       </c>
       <c r="E88">
-        <v>-3.1196662490986447E-4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.00031196662490986447</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>92</v>
       </c>
       <c r="B89">
-        <v>486.68179515704668</v>
+        <v>486.6817951570467</v>
       </c>
       <c r="C89">
-        <v>4.9635709795307935E-4</v>
+        <v>0.0004963570979530794</v>
       </c>
       <c r="D89">
-        <v>3.2004873590351111E-2</v>
+        <v>0.03200487359035111</v>
       </c>
       <c r="E89">
-        <v>-3.134651645689342E-5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.134651645689342e-5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>93</v>
       </c>
@@ -2475,33 +2470,33 @@
         <v>126.9767299474213</v>
       </c>
       <c r="C90">
-        <v>-1.6553680569102549E-4</v>
+        <v>-0.0001655368056910255</v>
       </c>
       <c r="D90">
-        <v>-2.4533559874365854E-2</v>
+        <v>-0.024533559874365854</v>
       </c>
       <c r="E90">
-        <v>2.4052914168587593E-5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.4052914168587593e-5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>94</v>
       </c>
       <c r="B91">
-        <v>84.701267450851859</v>
+        <v>84.70126745085186</v>
       </c>
       <c r="C91">
-        <v>2.5591359885793034E-4</v>
+        <v>0.00025591359885793034</v>
       </c>
       <c r="D91">
-        <v>2.4933921395914289E-2</v>
+        <v>0.02493392139591429</v>
       </c>
       <c r="E91">
-        <v>-2.4433808308527345E-5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-2.4433808308527345e-5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -2509,50 +2504,50 @@
         <v>0.30066254435730366</v>
       </c>
       <c r="C92">
-        <v>-2.851398607942417E-6</v>
+        <v>-2.851398607942417e-6</v>
       </c>
       <c r="D92">
-        <v>-3.1017548591837898E-4</v>
+        <v>-0.000310175485918379</v>
       </c>
       <c r="E92">
-        <v>3.0613332341107063E-7</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.0613332341107063e-7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>96</v>
       </c>
       <c r="B93">
-        <v>582.93357348816028</v>
+        <v>582.9335734881603</v>
       </c>
       <c r="C93">
-        <v>3.1237528626846486E-3</v>
+        <v>0.0031237528626846486</v>
       </c>
       <c r="D93">
-        <v>0.31783666233027408</v>
+        <v>0.3178366623302741</v>
       </c>
       <c r="E93">
-        <v>-3.1196662490986447E-4</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.00031196662490986447</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>97</v>
       </c>
       <c r="B94">
-        <v>486.68179515704668</v>
+        <v>486.6817951570467</v>
       </c>
       <c r="C94">
-        <v>4.9635709795307935E-4</v>
+        <v>0.0004963570979530794</v>
       </c>
       <c r="D94">
-        <v>3.2004873590351111E-2</v>
+        <v>0.03200487359035111</v>
       </c>
       <c r="E94">
-        <v>-3.134651645689342E-5</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.134651645689342e-5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>98</v>
       </c>
@@ -2560,33 +2555,33 @@
         <v>126.9767299474213</v>
       </c>
       <c r="C95">
-        <v>-1.6553680569102549E-4</v>
+        <v>-0.0001655368056910255</v>
       </c>
       <c r="D95">
-        <v>-2.4533559874365854E-2</v>
+        <v>-0.024533559874365854</v>
       </c>
       <c r="E95">
-        <v>2.4052914168587593E-5</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.4052914168587593e-5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>99</v>
       </c>
       <c r="B96">
-        <v>84.701267450851859</v>
+        <v>84.70126745085186</v>
       </c>
       <c r="C96">
-        <v>2.5591359885793034E-4</v>
+        <v>0.00025591359885793034</v>
       </c>
       <c r="D96">
-        <v>2.4933921395914289E-2</v>
+        <v>0.02493392139591429</v>
       </c>
       <c r="E96">
-        <v>-2.4433808308527345E-5</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-2.4433808308527345e-5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>100</v>
       </c>
@@ -2594,50 +2589,50 @@
         <v>0.30066254435730366</v>
       </c>
       <c r="C97">
-        <v>-2.851398607942417E-6</v>
+        <v>-2.851398607942417e-6</v>
       </c>
       <c r="D97">
-        <v>-3.1017548591837898E-4</v>
+        <v>-0.000310175485918379</v>
       </c>
       <c r="E97">
-        <v>3.0613332341107063E-7</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.0613332341107063e-7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>101</v>
       </c>
       <c r="B98">
-        <v>582.93357348816028</v>
+        <v>582.9335734881603</v>
       </c>
       <c r="C98">
-        <v>3.1237528626846486E-3</v>
+        <v>0.0031237528626846486</v>
       </c>
       <c r="D98">
-        <v>0.31783666233027408</v>
+        <v>0.3178366623302741</v>
       </c>
       <c r="E98">
-        <v>-3.1196662490986447E-4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.00031196662490986447</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>102</v>
       </c>
       <c r="B99">
-        <v>486.68179515704668</v>
+        <v>486.6817951570467</v>
       </c>
       <c r="C99">
-        <v>4.9635709795307935E-4</v>
+        <v>0.0004963570979530794</v>
       </c>
       <c r="D99">
-        <v>3.2004873590351111E-2</v>
+        <v>0.03200487359035111</v>
       </c>
       <c r="E99">
-        <v>-3.134651645689342E-5</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.134651645689342e-5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>103</v>
       </c>
@@ -2645,33 +2640,33 @@
         <v>126.9767299474213</v>
       </c>
       <c r="C100">
-        <v>-1.6553680569102549E-4</v>
+        <v>-0.0001655368056910255</v>
       </c>
       <c r="D100">
-        <v>-2.4533559874365854E-2</v>
+        <v>-0.024533559874365854</v>
       </c>
       <c r="E100">
-        <v>2.4052914168587593E-5</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.4052914168587593e-5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
         <v>104</v>
       </c>
       <c r="B101">
-        <v>84.701267450851859</v>
+        <v>84.70126745085186</v>
       </c>
       <c r="C101">
-        <v>2.5591359885793034E-4</v>
+        <v>0.00025591359885793034</v>
       </c>
       <c r="D101">
-        <v>2.4933921395914289E-2</v>
+        <v>0.02493392139591429</v>
       </c>
       <c r="E101">
-        <v>-2.4433808308527345E-5</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-2.4433808308527345e-5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
         <v>105</v>
       </c>
@@ -2679,50 +2674,50 @@
         <v>0.30066254435730366</v>
       </c>
       <c r="C102">
-        <v>-2.851398607942417E-6</v>
+        <v>-2.851398607942417e-6</v>
       </c>
       <c r="D102">
-        <v>-3.1017548591837898E-4</v>
+        <v>-0.000310175485918379</v>
       </c>
       <c r="E102">
-        <v>3.0613332341107063E-7</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.0613332341107063e-7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
         <v>106</v>
       </c>
       <c r="B103">
-        <v>582.93357348816028</v>
+        <v>582.9335734881603</v>
       </c>
       <c r="C103">
-        <v>3.1237528626846486E-3</v>
+        <v>0.0031237528626846486</v>
       </c>
       <c r="D103">
-        <v>0.31783666233027408</v>
+        <v>0.3178366623302741</v>
       </c>
       <c r="E103">
-        <v>-3.1196662490986447E-4</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.00031196662490986447</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
         <v>107</v>
       </c>
       <c r="B104">
-        <v>486.68179515704668</v>
+        <v>486.6817951570467</v>
       </c>
       <c r="C104">
-        <v>4.9635709795307935E-4</v>
+        <v>0.0004963570979530794</v>
       </c>
       <c r="D104">
-        <v>3.2004873590351111E-2</v>
+        <v>0.03200487359035111</v>
       </c>
       <c r="E104">
-        <v>-3.134651645689342E-5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.134651645689342e-5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" t="s">
         <v>108</v>
       </c>
@@ -2730,33 +2725,33 @@
         <v>126.9767299474213</v>
       </c>
       <c r="C105">
-        <v>-1.6553680569102549E-4</v>
+        <v>-0.0001655368056910255</v>
       </c>
       <c r="D105">
-        <v>-2.4533559874365854E-2</v>
+        <v>-0.024533559874365854</v>
       </c>
       <c r="E105">
-        <v>2.4052914168587593E-5</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.4052914168587593e-5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" t="s">
         <v>109</v>
       </c>
       <c r="B106">
-        <v>84.701267450851859</v>
+        <v>84.70126745085186</v>
       </c>
       <c r="C106">
-        <v>2.5591359885793034E-4</v>
+        <v>0.00025591359885793034</v>
       </c>
       <c r="D106">
-        <v>2.4933921395914289E-2</v>
+        <v>0.02493392139591429</v>
       </c>
       <c r="E106">
-        <v>-2.4433808308527345E-5</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-2.4433808308527345e-5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107" t="s">
         <v>110</v>
       </c>
@@ -2764,16 +2759,16 @@
         <v>0.30066254435730366</v>
       </c>
       <c r="C107">
-        <v>-2.851398607942417E-6</v>
+        <v>-2.851398607942417e-6</v>
       </c>
       <c r="D107">
-        <v>-3.1017548591837898E-4</v>
+        <v>-0.000310175485918379</v>
       </c>
       <c r="E107">
-        <v>3.0613332341107063E-7</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.0613332341107063e-7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" t="s">
         <v>111</v>
       </c>
@@ -2781,50 +2776,50 @@
         <v>464.63946108686514</v>
       </c>
       <c r="C108">
-        <v>3.2401614565962665E-3</v>
+        <v>0.0032401614565962665</v>
       </c>
       <c r="D108">
         <v>0.33653780018721086</v>
       </c>
       <c r="E108">
-        <v>-3.3030373853281742E-4</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.0003303037385328174</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" t="s">
         <v>112</v>
       </c>
       <c r="B109">
-        <v>604.97590755834187</v>
+        <v>604.9759075583419</v>
       </c>
       <c r="C109">
-        <v>3.7994850404140981E-4</v>
+        <v>0.0003799485040414098</v>
       </c>
       <c r="D109">
-        <v>1.3303613926337249E-2</v>
+        <v>0.013303613926337249</v>
       </c>
       <c r="E109">
-        <v>-1.3011101173552649E-5</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.3011101173552649e-5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
       <c r="A110" t="s">
         <v>113</v>
       </c>
       <c r="B110">
-        <v>8.6826175461261954</v>
+        <v>8.682617546126195</v>
       </c>
       <c r="C110">
-        <v>-4.9128209336013694E-5</v>
+        <v>-4.9128209336013694e-5</v>
       </c>
       <c r="D110">
-        <v>-5.8324093289729931E-3</v>
+        <v>-0.005832409328972993</v>
       </c>
       <c r="E110">
-        <v>5.7165435689216708E-6</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.716543568921671e-6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
         <v>114</v>
       </c>
@@ -2832,16 +2827,16 @@
         <v>202.99537985214695</v>
       </c>
       <c r="C111">
-        <v>1.3950501471996226E-4</v>
+        <v>0.00013950501471996226</v>
       </c>
       <c r="D111">
-        <v>6.2327936893092706E-3</v>
+        <v>0.006232793689309271</v>
       </c>
       <c r="E111">
-        <v>-6.0971192701454443E-6</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-6.097119270145444e-6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
       <c r="A112" t="s">
         <v>115</v>
       </c>
@@ -2849,16 +2844,16 @@
         <v>0.30066254435730366</v>
       </c>
       <c r="C112">
-        <v>-2.851398607942417E-6</v>
+        <v>-2.851398607942417e-6</v>
       </c>
       <c r="D112">
-        <v>-3.1017548591837898E-4</v>
+        <v>-0.000310175485918379</v>
       </c>
       <c r="E112">
-        <v>3.0613332341107063E-7</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.0613332341107063e-7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
         <v>116</v>
       </c>
@@ -2866,50 +2861,50 @@
         <v>464.63946108686514</v>
       </c>
       <c r="C113">
-        <v>3.2401614565962665E-3</v>
+        <v>0.0032401614565962665</v>
       </c>
       <c r="D113">
         <v>0.33653780018721086</v>
       </c>
       <c r="E113">
-        <v>-3.3030373853281742E-4</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.0003303037385328174</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
         <v>117</v>
       </c>
       <c r="B114">
-        <v>604.97590755834187</v>
+        <v>604.9759075583419</v>
       </c>
       <c r="C114">
-        <v>3.7994850404140981E-4</v>
+        <v>0.0003799485040414098</v>
       </c>
       <c r="D114">
-        <v>1.3303613926337249E-2</v>
+        <v>0.013303613926337249</v>
       </c>
       <c r="E114">
-        <v>-1.3011101173552649E-5</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.3011101173552649e-5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
         <v>118</v>
       </c>
       <c r="B115">
-        <v>8.6826175461261954</v>
+        <v>8.682617546126195</v>
       </c>
       <c r="C115">
-        <v>-4.9128209336013694E-5</v>
+        <v>-4.9128209336013694e-5</v>
       </c>
       <c r="D115">
-        <v>-5.8324093289729931E-3</v>
+        <v>-0.005832409328972993</v>
       </c>
       <c r="E115">
-        <v>5.7165435689216708E-6</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.716543568921671e-6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
         <v>119</v>
       </c>
@@ -2917,16 +2912,16 @@
         <v>202.99537985214695</v>
       </c>
       <c r="C116">
-        <v>1.3950501471996226E-4</v>
+        <v>0.00013950501471996226</v>
       </c>
       <c r="D116">
-        <v>6.2327936893092706E-3</v>
+        <v>0.006232793689309271</v>
       </c>
       <c r="E116">
-        <v>-6.0971192701454443E-6</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-6.097119270145444e-6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
         <v>120</v>
       </c>
@@ -2934,16 +2929,16 @@
         <v>0.30066254435730366</v>
       </c>
       <c r="C117">
-        <v>-2.851398607942417E-6</v>
+        <v>-2.851398607942417e-6</v>
       </c>
       <c r="D117">
-        <v>-3.1017548591837898E-4</v>
+        <v>-0.000310175485918379</v>
       </c>
       <c r="E117">
-        <v>3.0613332341107063E-7</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.0613332341107063e-7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
         <v>121</v>
       </c>
@@ -2951,50 +2946,50 @@
         <v>464.63946108686514</v>
       </c>
       <c r="C118">
-        <v>3.2401614565962665E-3</v>
+        <v>0.0032401614565962665</v>
       </c>
       <c r="D118">
         <v>0.33653780018721086</v>
       </c>
       <c r="E118">
-        <v>-3.3030373853281742E-4</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.0003303037385328174</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
       <c r="A119" t="s">
         <v>122</v>
       </c>
       <c r="B119">
-        <v>604.97590755834187</v>
+        <v>604.9759075583419</v>
       </c>
       <c r="C119">
-        <v>3.7994850404140981E-4</v>
+        <v>0.0003799485040414098</v>
       </c>
       <c r="D119">
-        <v>1.3303613926337249E-2</v>
+        <v>0.013303613926337249</v>
       </c>
       <c r="E119">
-        <v>-1.3011101173552649E-5</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.3011101173552649e-5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
       <c r="A120" t="s">
         <v>123</v>
       </c>
       <c r="B120">
-        <v>8.6826175461261954</v>
+        <v>8.682617546126195</v>
       </c>
       <c r="C120">
-        <v>-4.9128209336013694E-5</v>
+        <v>-4.9128209336013694e-5</v>
       </c>
       <c r="D120">
-        <v>-5.8324093289729931E-3</v>
+        <v>-0.005832409328972993</v>
       </c>
       <c r="E120">
-        <v>5.7165435689216708E-6</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.716543568921671e-6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
       <c r="A121" t="s">
         <v>124</v>
       </c>
@@ -3002,16 +2997,16 @@
         <v>202.99537985214695</v>
       </c>
       <c r="C121">
-        <v>1.3950501471996226E-4</v>
+        <v>0.00013950501471996226</v>
       </c>
       <c r="D121">
-        <v>6.2327936893092706E-3</v>
+        <v>0.006232793689309271</v>
       </c>
       <c r="E121">
-        <v>-6.0971192701454443E-6</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-6.097119270145444e-6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
       <c r="A122" t="s">
         <v>125</v>
       </c>
@@ -3019,16 +3014,16 @@
         <v>0.30066254435730366</v>
       </c>
       <c r="C122">
-        <v>-2.851398607942417E-6</v>
+        <v>-2.851398607942417e-6</v>
       </c>
       <c r="D122">
-        <v>-3.1017548591837898E-4</v>
+        <v>-0.000310175485918379</v>
       </c>
       <c r="E122">
-        <v>3.0613332341107063E-7</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.0613332341107063e-7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
         <v>126</v>
       </c>
@@ -3036,50 +3031,50 @@
         <v>464.63946108686514</v>
       </c>
       <c r="C123">
-        <v>3.2401614565962665E-3</v>
+        <v>0.0032401614565962665</v>
       </c>
       <c r="D123">
         <v>0.33653780018721086</v>
       </c>
       <c r="E123">
-        <v>-3.3030373853281742E-4</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.0003303037385328174</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
       <c r="A124" t="s">
         <v>127</v>
       </c>
       <c r="B124">
-        <v>604.97590755834187</v>
+        <v>604.9759075583419</v>
       </c>
       <c r="C124">
-        <v>3.7994850404140981E-4</v>
+        <v>0.0003799485040414098</v>
       </c>
       <c r="D124">
-        <v>1.3303613926337249E-2</v>
+        <v>0.013303613926337249</v>
       </c>
       <c r="E124">
-        <v>-1.3011101173552649E-5</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.3011101173552649e-5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
       <c r="A125" t="s">
         <v>128</v>
       </c>
       <c r="B125">
-        <v>8.6826175461261954</v>
+        <v>8.682617546126195</v>
       </c>
       <c r="C125">
-        <v>-4.9128209336013694E-5</v>
+        <v>-4.9128209336013694e-5</v>
       </c>
       <c r="D125">
-        <v>-5.8324093289729931E-3</v>
+        <v>-0.005832409328972993</v>
       </c>
       <c r="E125">
-        <v>5.7165435689216708E-6</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.716543568921671e-6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
         <v>129</v>
       </c>
@@ -3087,16 +3082,16 @@
         <v>202.99537985214695</v>
       </c>
       <c r="C126">
-        <v>1.3950501471996226E-4</v>
+        <v>0.00013950501471996226</v>
       </c>
       <c r="D126">
-        <v>6.2327936893092706E-3</v>
+        <v>0.006232793689309271</v>
       </c>
       <c r="E126">
-        <v>-6.0971192701454443E-6</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-6.097119270145444e-6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
         <v>130</v>
       </c>
@@ -3104,186 +3099,186 @@
         <v>463.34597144451664</v>
       </c>
       <c r="C127">
-        <v>3.2394243375312194E-3</v>
+        <v>0.0032394243375312194</v>
       </c>
       <c r="D127">
-        <v>0.33651680477240109</v>
+        <v>0.3365168047724011</v>
       </c>
       <c r="E127">
-        <v>-3.3029178451269789E-4</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.0003302917845126979</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
       <c r="A128" t="s">
         <v>131</v>
       </c>
       <c r="B128">
-        <v>3.6744648701291255E-10</v>
+        <v>3.6744648701291255e-10</v>
       </c>
       <c r="C128">
-        <v>-3.695017194905453E-15</v>
+        <v>-3.695017194905453e-15</v>
       </c>
       <c r="D128">
-        <v>-3.850984010421278E-13</v>
+        <v>-3.850984010421278e-13</v>
       </c>
       <c r="E128">
-        <v>3.8002002270167146E-16</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.8002002270167146e-16</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
       <c r="A129" t="s">
         <v>132</v>
       </c>
       <c r="B129">
-        <v>0.99999900158136901</v>
+        <v>0.999999001581369</v>
       </c>
       <c r="C129">
-        <v>1.5271297772596267E-13</v>
+        <v>1.5271297772596267e-13</v>
       </c>
       <c r="D129">
-        <v>2.379040710097595E-10</v>
+        <v>2.379040710097595e-10</v>
       </c>
       <c r="E129">
-        <v>6.6341390224642549E-12</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6.634139022464255e-12</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
       <c r="A130" t="s">
         <v>133</v>
       </c>
       <c r="B130">
-        <v>7.3935472220173544E-7</v>
+        <v>7.393547222017354e-7</v>
       </c>
       <c r="C130">
-        <v>4.1273665806713616E-14</v>
+        <v>4.1273665806713616e-14</v>
       </c>
       <c r="D130">
-        <v>4.1371940556074246E-12</v>
+        <v>4.137194055607425e-12</v>
       </c>
       <c r="E130">
-        <v>-4.0536315550996648E-15</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-4.053631555099665e-15</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
       <c r="A131" t="s">
         <v>134</v>
       </c>
       <c r="B131">
-        <v>1.0611223031523729E-8</v>
+        <v>1.0611223031523729e-8</v>
       </c>
       <c r="C131">
-        <v>-6.6112596300824743E-14</v>
+        <v>-6.611259630082474e-14</v>
       </c>
       <c r="D131">
-        <v>-7.3019198435236023E-12</v>
+        <v>-7.301919843523602e-12</v>
       </c>
       <c r="E131">
-        <v>7.156332774549773E-15</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.156332774549773e-15</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
       <c r="A132" t="s">
         <v>135</v>
       </c>
       <c r="B132">
-        <v>2.4808523910408143E-7</v>
+        <v>2.4808523910408143e-7</v>
       </c>
       <c r="C132">
-        <v>2.8534073273718374E-14</v>
+        <v>2.8534073273718374e-14</v>
       </c>
       <c r="D132">
-        <v>3.5499059843691758E-12</v>
+        <v>3.5499059843691758e-12</v>
       </c>
       <c r="E132">
-        <v>-3.4784009107192957E-15</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.4784009107192957e-15</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
       <c r="A133" t="s">
         <v>136</v>
       </c>
       <c r="B133">
-        <v>818.24805714332092</v>
+        <v>818.2480571433209</v>
       </c>
       <c r="C133">
-        <v>4.6821093256607112E-4</v>
+        <v>0.0004682109325660711</v>
       </c>
       <c r="D133">
-        <v>1.3414677732467266E-2</v>
+        <v>0.013414677732467266</v>
       </c>
       <c r="E133">
-        <v>-1.3107103803341968E-5</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.3107103803341968e-5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
       <c r="A134" t="s">
         <v>137</v>
       </c>
       <c r="B134">
-        <v>3.6744648701291253E-4</v>
+        <v>0.00036744648701291253</v>
       </c>
       <c r="C134">
-        <v>-3.6950171706111338E-9</v>
+        <v>-3.6950171706111338e-9</v>
       </c>
       <c r="D134">
-        <v>-3.8509837759505263E-7</v>
+        <v>-3.850983775950526e-7</v>
       </c>
       <c r="E134">
-        <v>3.8001943539597241E-10</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.800194353959724e-10</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
       <c r="A135" t="s">
         <v>138</v>
       </c>
       <c r="B135">
-        <v>1.5813691756464694E-3</v>
+        <v>0.0015813691756464694</v>
       </c>
       <c r="C135">
-        <v>-5.1003735079343927E-14</v>
+        <v>-5.1003735079343927e-14</v>
       </c>
       <c r="D135">
-        <v>-2.4162232769585173E-11</v>
+        <v>-2.4162232769585173e-11</v>
       </c>
       <c r="E135">
-        <v>1.2957313907837354E-14</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.2957313907837354e-14</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
       <c r="A136" t="s">
         <v>139</v>
       </c>
       <c r="B136">
-        <v>0.73935472220173548</v>
+        <v>0.7393547222017355</v>
       </c>
       <c r="C136">
-        <v>4.1273644811454753E-8</v>
+        <v>4.127364481145475e-8</v>
       </c>
       <c r="D136">
-        <v>4.137208750795445E-6</v>
+        <v>4.137208750795445e-6</v>
       </c>
       <c r="E136">
-        <v>-4.0531705589854741E-9</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-4.053170558985474e-9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
       <c r="A137" t="s">
         <v>140</v>
       </c>
       <c r="B137">
-        <v>1.0611223031523729E-2</v>
+        <v>0.01061122303152373</v>
       </c>
       <c r="C137">
-        <v>-6.6112596667760748E-8</v>
+        <v>-6.611259666776075e-8</v>
       </c>
       <c r="D137">
-        <v>-7.3019190616023606E-6</v>
+        <v>-7.301919061602361e-6</v>
       </c>
       <c r="E137">
-        <v>7.1563482594065448E-9</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.156348259406545e-9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
       <c r="A138" t="s">
         <v>141</v>
       </c>
@@ -3291,16 +3286,16 @@
         <v>0.2480852391040814</v>
       </c>
       <c r="C138">
-        <v>2.8534106118092086E-8</v>
+        <v>2.8534106118092086e-8</v>
       </c>
       <c r="D138">
-        <v>3.5499114946922771E-6</v>
+        <v>3.549911494692277e-6</v>
       </c>
       <c r="E138">
-        <v>-3.4772643122346917E-9</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.4772643122346917e-9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
       <c r="A139" t="s">
         <v>142</v>
       </c>
@@ -3308,16 +3303,16 @@
         <v>0.30066237410245417</v>
       </c>
       <c r="C139">
-        <v>-2.8513980947820799E-6</v>
+        <v>-2.85139809478208e-6</v>
       </c>
       <c r="D139">
-        <v>-3.1017543117581173E-4</v>
+        <v>-0.00031017543117581173</v>
       </c>
       <c r="E139">
-        <v>3.0613326870359305E-7</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.0613326870359305e-7</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
       <c r="A140" t="s">
         <v>143</v>
       </c>
@@ -3325,50 +3320,50 @@
         <v>1.2939522555990586</v>
       </c>
       <c r="C140">
-        <v>7.403725391180017E-7</v>
+        <v>7.403725391180017e-7</v>
       </c>
       <c r="D140">
-        <v>2.119371666607169E-5</v>
+        <v>2.119371666607169e-5</v>
       </c>
       <c r="E140">
-        <v>-2.0722439448492282E-8</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-2.0722439448492282e-8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
       <c r="A141" t="s">
         <v>144</v>
       </c>
       <c r="B141">
-        <v>604.97556498130984</v>
+        <v>604.9755649813098</v>
       </c>
       <c r="C141">
-        <v>3.7994607829758335E-4</v>
+        <v>0.00037994607829758335</v>
       </c>
       <c r="D141">
-        <v>1.3303525625987318E-2</v>
+        <v>0.013303525625987318</v>
       </c>
       <c r="E141">
-        <v>-1.3010855069565421E-5</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.3010855069565421e-5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
       <c r="A142" t="s">
         <v>145</v>
       </c>
       <c r="B142">
-        <v>8.6826126294587525</v>
+        <v>8.682612629458752</v>
       </c>
       <c r="C142">
-        <v>-4.9128212999838661E-5</v>
+        <v>-4.912821299983866e-5</v>
       </c>
       <c r="D142">
-        <v>-5.8324107859791747E-3</v>
+        <v>-0.005832410785979175</v>
       </c>
       <c r="E142">
-        <v>5.7164906803883886E-6</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.716490680388389e-6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
       <c r="A143" t="s">
         <v>146</v>
       </c>
@@ -3376,84 +3371,84 @@
         <v>202.99526490285083</v>
       </c>
       <c r="C143">
-        <v>1.3950419308003082E-4</v>
+        <v>0.00013950419308003082</v>
       </c>
       <c r="D143">
-        <v>6.2326882626258309E-3</v>
+        <v>0.006232688262625831</v>
       </c>
       <c r="E143">
-        <v>-6.0978848786010869E-6</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-6.097884878601087e-6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
       <c r="A144" t="s">
         <v>147</v>
       </c>
       <c r="B144">
-        <v>3.0066237410245419E-4</v>
+        <v>0.0003006623741024542</v>
       </c>
       <c r="C144">
-        <v>-2.8513981079058764E-9</v>
+        <v>-2.8513981079058764e-9</v>
       </c>
       <c r="D144">
-        <v>-3.1017544418615098E-7</v>
+        <v>-3.10175444186151e-7</v>
       </c>
       <c r="E144">
-        <v>3.0613289294177666E-10</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.0613289294177666e-10</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
       <c r="A145" t="s">
         <v>148</v>
       </c>
       <c r="B145">
-        <v>1.2939522555990585E-3</v>
+        <v>0.0012939522555990585</v>
       </c>
       <c r="C145">
-        <v>7.4037257371710842E-10</v>
+        <v>7.403725737171084e-10</v>
       </c>
       <c r="D145">
-        <v>2.1193778619659082E-8</v>
+        <v>2.1193778619659082e-8</v>
       </c>
       <c r="E145">
-        <v>-2.0717204698031633E-11</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-2.0717204698031633e-11</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
       <c r="A146" t="s">
         <v>149</v>
       </c>
       <c r="B146">
-        <v>586.82629803187058</v>
+        <v>586.8262980318706</v>
       </c>
       <c r="C146">
-        <v>3.6854765294469299E-4</v>
+        <v>0.000368547652944693</v>
       </c>
       <c r="D146">
-        <v>1.2904404428447367E-2</v>
+        <v>0.012904404428447367</v>
       </c>
       <c r="E146">
-        <v>-1.2623110893488749E-5</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.2623110893488749e-5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
       <c r="A147" t="s">
         <v>150</v>
       </c>
       <c r="B147">
-        <v>8.6826126294587535E-3</v>
+        <v>0.008682612629458753</v>
       </c>
       <c r="C147">
-        <v>-4.9128214126097448E-8</v>
+        <v>-4.912821412609745e-8</v>
       </c>
       <c r="D147">
-        <v>-5.8324103002549077E-6</v>
+        <v>-5.832410300254908e-6</v>
       </c>
       <c r="E147">
-        <v>5.7164442414195553E-9</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.716444241419555e-9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
       <c r="A148" t="s">
         <v>151</v>
       </c>
@@ -3461,33 +3456,33 @@
         <v>0.20299526490285083</v>
       </c>
       <c r="C148">
-        <v>1.3950420835132755E-7</v>
+        <v>1.3950420835132755e-7</v>
       </c>
       <c r="D148">
-        <v>6.2326909588743625E-6</v>
+        <v>6.2326909588743625e-6</v>
       </c>
       <c r="E148">
-        <v>-6.0973541475402977E-9</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-6.097354147540298e-9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
       <c r="A149" t="s">
         <v>152</v>
       </c>
       <c r="B149">
-        <v>0.30036171172835169</v>
+        <v>0.3003617117283517</v>
       </c>
       <c r="C149">
-        <v>-2.8485466929458452E-6</v>
+        <v>-2.848546692945845e-6</v>
       </c>
       <c r="D149">
-        <v>-3.0986523040786834E-4</v>
+        <v>-0.00030986523040786834</v>
       </c>
       <c r="E149">
-        <v>3.0582708236189036E-7</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.0582708236189036e-7</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
       <c r="A150" t="s">
         <v>153</v>
       </c>
@@ -3495,16 +3490,16 @@
         <v>1.2926583033434595</v>
       </c>
       <c r="C150">
-        <v>7.3963217146571089E-7</v>
+        <v>7.396321714657109e-7</v>
       </c>
       <c r="D150">
-        <v>2.1172507089065867E-5</v>
+        <v>2.1172507089065867e-5</v>
       </c>
       <c r="E150">
-        <v>-2.0701663935929357E-8</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-2.0701663935929357e-8</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
       <c r="A151" t="s">
         <v>154</v>
       </c>
@@ -3512,33 +3507,33 @@
         <v>18.149266949439312</v>
       </c>
       <c r="C151">
-        <v>1.1398381371564244E-5</v>
+        <v>1.1398381371564244e-5</v>
       </c>
       <c r="D151">
-        <v>3.9910597179003155E-4</v>
+        <v>0.00039910597179003155</v>
       </c>
       <c r="E151">
-        <v>-3.902916852976522E-7</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.902916852976522e-7</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
       <c r="A152" t="s">
         <v>155</v>
       </c>
       <c r="B152">
-        <v>8.6739300168292939</v>
+        <v>8.673930016829294</v>
       </c>
       <c r="C152">
-        <v>-4.9079084993306551E-5</v>
+        <v>-4.907908499330655e-5</v>
       </c>
       <c r="D152">
-        <v>-5.8265786073877415E-3</v>
+        <v>-0.0058265786073877415</v>
       </c>
       <c r="E152">
-        <v>5.710765114206288E-6</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.710765114206288e-6</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
       <c r="A153" t="s">
         <v>156</v>
       </c>
@@ -3546,33 +3541,33 @@
         <v>202.79226963794798</v>
       </c>
       <c r="C153">
-        <v>1.3936469230772596E-4</v>
+        <v>0.00013936469230772596</v>
       </c>
       <c r="D153">
-        <v>6.2264563051855886E-3</v>
+        <v>0.006226456305185589</v>
       </c>
       <c r="E153">
-        <v>-6.0917742561568159E-6</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-6.091774256156816e-6</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
       <c r="A154" t="s">
         <v>157</v>
       </c>
       <c r="B154">
-        <v>311</v>
+        <v>311.0</v>
       </c>
       <c r="C154">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D154">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="E154">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
       <c r="A155" t="s">
         <v>158</v>
       </c>
@@ -3580,33 +3575,33 @@
         <v>397.24612753336663</v>
       </c>
       <c r="C155">
-        <v>8.6547707164815079E-5</v>
+        <v>8.654770716481508e-5</v>
       </c>
       <c r="D155">
-        <v>9.5151303478169559E-3</v>
+        <v>0.009515130347816956</v>
       </c>
       <c r="E155">
-        <v>-9.3713703740449868E-6</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-9.371370374044987e-6</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
       <c r="A156" t="s">
         <v>159</v>
       </c>
       <c r="B156">
-        <v>423</v>
+        <v>423.0</v>
       </c>
       <c r="C156">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="D156">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="E156">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
       <c r="A157" t="s">
         <v>160</v>
       </c>
@@ -3614,118 +3609,118 @@
         <v>397.24612753336663</v>
       </c>
       <c r="C157">
-        <v>8.6547707164815079E-5</v>
+        <v>8.654770716481508e-5</v>
       </c>
       <c r="D157">
-        <v>9.5151303478169559E-3</v>
+        <v>0.009515130347816956</v>
       </c>
       <c r="E157">
-        <v>-9.3713703740449868E-6</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-9.371370374044987e-6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
       <c r="A158" t="s">
         <v>161</v>
       </c>
       <c r="B158">
-        <v>644.59531650062831</v>
+        <v>644.5953165006283</v>
       </c>
       <c r="C158">
-        <v>2.6654204647555803E-7</v>
+        <v>2.6654204647555803e-7</v>
       </c>
       <c r="D158">
-        <v>-4.9036084968925387E-4</v>
+        <v>-0.0004903608496892539</v>
       </c>
       <c r="E158">
-        <v>2.5865733887512611E-7</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.586573388751261e-7</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
       <c r="A159" t="s">
         <v>162</v>
       </c>
       <c r="B159">
-        <v>609.20000017064842</v>
+        <v>609.2000001706484</v>
       </c>
       <c r="C159">
-        <v>-9.203628341727306E-5</v>
+        <v>-9.203628341727306e-5</v>
       </c>
       <c r="D159">
-        <v>-1.0474326311733013E-2</v>
+        <v>-0.010474326311733013</v>
       </c>
       <c r="E159">
-        <v>1.0129740100090409E-5</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.0129740100090409e-5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
       <c r="A160" t="s">
         <v>163</v>
       </c>
       <c r="B160">
-        <v>609.20000034718782</v>
+        <v>609.2000003471878</v>
       </c>
       <c r="C160">
-        <v>-1.1261939985296618E-4</v>
+        <v>-0.00011261939985296618</v>
       </c>
       <c r="D160">
-        <v>-1.0474789827675799E-2</v>
+        <v>-0.0104747898276758</v>
       </c>
       <c r="E160">
-        <v>1.0075449927550787E-5</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.0075449927550787e-5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
       <c r="A161" t="s">
         <v>164</v>
       </c>
       <c r="B161">
-        <v>609.20000034718782</v>
+        <v>609.2000003471878</v>
       </c>
       <c r="C161">
-        <v>-1.1261939985296618E-4</v>
+        <v>-0.00011261939985296618</v>
       </c>
       <c r="D161">
-        <v>-1.0474789827675799E-2</v>
+        <v>-0.0104747898276758</v>
       </c>
       <c r="E161">
-        <v>1.0075449927550787E-5</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.0075449927550787e-5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
       <c r="A162" t="s">
         <v>165</v>
       </c>
       <c r="B162">
-        <v>951.48240810154016</v>
+        <v>951.4824081015402</v>
       </c>
       <c r="C162">
-        <v>2.9550040167310714E-5</v>
+        <v>2.9550040167310714e-5</v>
       </c>
       <c r="D162">
-        <v>-2.8899458167839365E-4</v>
+        <v>-0.00028899458167839365</v>
       </c>
       <c r="E162">
-        <v>1.6475887447553207E-7</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.6475887447553207e-7</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
       <c r="A163" t="s">
         <v>166</v>
       </c>
       <c r="B163">
-        <v>951.48240810154016</v>
+        <v>951.4824081015402</v>
       </c>
       <c r="C163">
-        <v>2.9550040167310714E-5</v>
+        <v>2.9550040167310714e-5</v>
       </c>
       <c r="D163">
-        <v>-2.8899458167839365E-4</v>
+        <v>-0.00028899458167839365</v>
       </c>
       <c r="E163">
-        <v>1.6475887447553207E-7</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.6475887447553207e-7</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
       <c r="A164" t="s">
         <v>167</v>
       </c>
@@ -3733,33 +3728,33 @@
         <v>1291.817465833818</v>
       </c>
       <c r="C164">
-        <v>5.573264255045872E-6</v>
+        <v>5.573264255045872e-6</v>
       </c>
       <c r="D164">
-        <v>-3.2743778048596466E-3</v>
+        <v>-0.0032743778048596466</v>
       </c>
       <c r="E164">
-        <v>2.8822564879528025E-6</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.8822564879528025e-6</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
       <c r="A165" t="s">
         <v>168</v>
       </c>
       <c r="B165">
-        <v>634.20000050571946</v>
+        <v>634.2000005057195</v>
       </c>
       <c r="C165">
-        <v>-1.7598092892166919E-4</v>
+        <v>-0.0001759809289216692</v>
       </c>
       <c r="D165">
-        <v>-1.0475709676457223E-2</v>
+        <v>-0.010475709676457223</v>
       </c>
       <c r="E165">
-        <v>1.0052333800568356E-5</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.0052333800568356e-5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
       <c r="A166" t="s">
         <v>169</v>
       </c>
@@ -3767,16 +3762,16 @@
         <v>293.00000003068044</v>
       </c>
       <c r="C166">
-        <v>-5.8641768814979361E-10</v>
+        <v>-5.864176881497936e-10</v>
       </c>
       <c r="D166">
-        <v>-2.8421707989590313E-7</v>
+        <v>-2.8421707989590313e-7</v>
       </c>
       <c r="E166">
-        <v>-1.268269837976284E-17</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.268269837976284e-17</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
       <c r="A167" t="s">
         <v>170</v>
       </c>
@@ -3784,16 +3779,16 @@
         <v>293.00000003068044</v>
       </c>
       <c r="C167">
-        <v>-5.8641768814979361E-10</v>
+        <v>-5.864176881497936e-10</v>
       </c>
       <c r="D167">
-        <v>-2.8421707989590313E-7</v>
+        <v>-2.8421707989590313e-7</v>
       </c>
       <c r="E167">
-        <v>-1.268269837976284E-17</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.268269837976284e-17</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
       <c r="A168" t="s">
         <v>171</v>
       </c>
@@ -3801,16 +3796,16 @@
         <v>293.00000003068044</v>
       </c>
       <c r="C168">
-        <v>-5.8641768814979361E-10</v>
+        <v>-5.864176881497936e-10</v>
       </c>
       <c r="D168">
-        <v>-2.8421707989590313E-7</v>
+        <v>-2.8421707989590313e-7</v>
       </c>
       <c r="E168">
-        <v>-1.268269837976284E-17</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.268269837976284e-17</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
       <c r="A169" t="s">
         <v>172</v>
       </c>
@@ -3818,16 +3813,16 @@
         <v>293.00000003068044</v>
       </c>
       <c r="C169">
-        <v>-5.8641768814979361E-10</v>
+        <v>-5.864176881497936e-10</v>
       </c>
       <c r="D169">
-        <v>-2.8421707989590313E-7</v>
+        <v>-2.8421707989590313e-7</v>
       </c>
       <c r="E169">
-        <v>-1.268269837976284E-17</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.268269837976284e-17</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
       <c r="A170" t="s">
         <v>173</v>
       </c>
@@ -3835,16 +3830,16 @@
         <v>293.00000003068044</v>
       </c>
       <c r="C170">
-        <v>-5.8641768814979361E-10</v>
+        <v>-5.864176881497936e-10</v>
       </c>
       <c r="D170">
-        <v>-2.8421707989590313E-7</v>
+        <v>-2.8421707989590313e-7</v>
       </c>
       <c r="E170">
-        <v>-1.268269837976284E-17</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.268269837976284e-17</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
       <c r="A171" t="s">
         <v>174</v>
       </c>
@@ -3852,16 +3847,16 @@
         <v>293.00000003068044</v>
       </c>
       <c r="C171">
-        <v>-5.8641768814979361E-10</v>
+        <v>-5.864176881497936e-10</v>
       </c>
       <c r="D171">
-        <v>-2.8421707989590313E-7</v>
+        <v>-2.8421707989590313e-7</v>
       </c>
       <c r="E171">
-        <v>-1.268269837976284E-17</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.268269837976284e-17</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
       <c r="A172" t="s">
         <v>175</v>
       </c>
@@ -3869,21 +3864,21 @@
         <v>293.00000003068044</v>
       </c>
       <c r="C172">
-        <v>-5.8641768814979361E-10</v>
+        <v>-5.864176881497936e-10</v>
       </c>
       <c r="D172">
-        <v>-2.8421707989590313E-7</v>
+        <v>-2.8421707989590313e-7</v>
       </c>
       <c r="E172">
-        <v>-1.268269837976284E-17</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.268269837976284e-17</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
       <c r="A173" t="s">
         <v>176</v>
       </c>
       <c r="B173">
-        <v>8520619.7885459159</v>
+        <v>8.520619788545916e6</v>
       </c>
       <c r="C173">
         <v>28.333624069470776</v>
@@ -3895,126 +3890,126 @@
         <v>-2.6692718576378596</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5">
       <c r="A174" t="s">
         <v>177</v>
       </c>
       <c r="B174">
-        <v>6.4455188518803943E-3</v>
+        <v>0.006445518851880394</v>
       </c>
       <c r="C174">
-        <v>-0.75151391373078569</v>
+        <v>-0.7515139137307857</v>
       </c>
       <c r="D174">
-        <v>-3.9532665794676514E-3</v>
+        <v>-0.003953266579467651</v>
       </c>
       <c r="E174">
-        <v>-1.7476453405266836E-3</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.0017476453405266836</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
       <c r="A175" t="s">
         <v>178</v>
       </c>
       <c r="B175">
-        <v>30741855.963244434</v>
+        <v>3.0741855963244434e7</v>
       </c>
       <c r="C175">
         <v>105.68875347588651</v>
       </c>
       <c r="D175">
-        <v>9666.8495780470712</v>
+        <v>9666.849578047071</v>
       </c>
       <c r="E175">
-        <v>-9.4940442658395909</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-9.494044265839591</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
       <c r="A176" t="s">
         <v>179</v>
       </c>
       <c r="B176">
-        <v>-30741855.963244434</v>
+        <v>-3.0741855963244434e7</v>
       </c>
       <c r="C176">
         <v>-105.68875347588651</v>
       </c>
       <c r="D176">
-        <v>-9666.8495780470712</v>
+        <v>-9666.849578047071</v>
       </c>
       <c r="E176">
-        <v>9.4940442658395909</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9.494044265839591</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
       <c r="A177" t="s">
         <v>180</v>
       </c>
       <c r="B177">
-        <v>-11511342.642409405</v>
+        <v>-1.1511342642409405e7</v>
       </c>
       <c r="C177">
-        <v>-9.1334834935013021</v>
+        <v>-9.133483493501302</v>
       </c>
       <c r="D177">
-        <v>-852.23433361927141</v>
+        <v>-852.2343336192714</v>
       </c>
       <c r="E177">
-        <v>0.83948920957210571</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.8394892095721057</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
       <c r="A178" t="s">
         <v>181</v>
       </c>
       <c r="B178">
-        <v>-7658230.168887455</v>
+        <v>-7.658230168887455e6</v>
       </c>
       <c r="C178">
         <v>-22.357280238825265</v>
       </c>
       <c r="D178">
-        <v>-2114.5395896807108</v>
+        <v>-2114.539589680711</v>
       </c>
       <c r="E178">
-        <v>2.0815869405328509</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.081586940532851</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
       <c r="A179" t="s">
         <v>182</v>
       </c>
       <c r="B179">
-        <v>716.82199382956378</v>
+        <v>716.8219938295638</v>
       </c>
       <c r="C179">
-        <v>3.4684914754603167E-3</v>
+        <v>0.0034684914754603167</v>
       </c>
       <c r="D179">
         <v>0.34907069314935024</v>
       </c>
       <c r="E179">
-        <v>-3.4258103152575114E-4</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.00034258103152575114</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
       <c r="A180" t="s">
         <v>183</v>
       </c>
       <c r="B180">
-        <v>556.99921340842491</v>
+        <v>556.9992134084249</v>
       </c>
       <c r="C180">
-        <v>4.1320122785283342</v>
+        <v>4.132012278528334</v>
       </c>
       <c r="D180">
-        <v>3.1534872749622903E-3</v>
+        <v>0.0031534872749622903</v>
       </c>
       <c r="E180">
-        <v>-3.0610654032265502E-6</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.06106540322655e-6</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
       <c r="A181" t="s">
         <v>184</v>
       </c>
@@ -4022,16 +4017,16 @@
         <v>29.827084623445646</v>
       </c>
       <c r="C181">
-        <v>-4.1316437308289649</v>
+        <v>-4.131643730828965</v>
       </c>
       <c r="D181">
-        <v>9.7509095402475727E-3</v>
+        <v>0.009750909540247573</v>
       </c>
       <c r="E181">
-        <v>-9.561833197568391E-6</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-9.561833197568391e-6</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
       <c r="A182" t="s">
         <v>185</v>
       </c>
@@ -4039,50 +4034,50 @@
         <v>145.39999996064918</v>
       </c>
       <c r="C182">
-        <v>6.0035248187718326E-5</v>
+        <v>6.0035248187718326e-5</v>
       </c>
       <c r="D182">
-        <v>6.1874011414018613E-5</v>
+        <v>6.187401141401861e-5</v>
       </c>
       <c r="E182">
-        <v>-5.0759019095006141E-8</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-5.075901909500614e-8</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
       <c r="A183" t="s">
         <v>186</v>
       </c>
       <c r="B183">
-        <v>3.9350816723423464E-8</v>
+        <v>3.9350816723423464e-8</v>
       </c>
       <c r="C183">
-        <v>0.99993996474474456</v>
+        <v>0.9999399647447446</v>
       </c>
       <c r="D183">
-        <v>-6.1862559661104595E-5</v>
+        <v>-6.18625596611046e-5</v>
       </c>
       <c r="E183">
-        <v>5.1225662122239735E-8</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.1225662122239735e-8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
       <c r="A184" t="s">
         <v>187</v>
       </c>
       <c r="B184">
-        <v>1.3897313754221703E-7</v>
+        <v>1.3897313754221703e-7</v>
       </c>
       <c r="C184">
-        <v>3.5314335463770088</v>
+        <v>3.531433546377009</v>
       </c>
       <c r="D184">
-        <v>-2.1847663475251352E-4</v>
+        <v>-0.00021847663475251352</v>
       </c>
       <c r="E184">
-        <v>1.8091088268521238E-7</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.8091088268521238e-7</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
       <c r="A185" t="s">
         <v>188</v>
       </c>
@@ -4093,10 +4088,10 @@
         <v>3.5315331214501007</v>
       </c>
       <c r="D185">
-        <v>2.9180858008252949E-4</v>
+        <v>0.0002918085800825295</v>
       </c>
       <c r="E185">
-        <v>-3.053720802971955E-7</v>
+        <v>-3.053720802971955e-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>